<commit_message>
Hex hovering, some work on still-bugged point to hex ocnversion
 Changes to be committed:
	modified:   SettleGame.xlsx
	modified:   app/__init__.pyc
	modified:   app/static/js/main.js
	modified:   app/static/js/main.ts
	modified:   app/views.pyc
</commit_message>
<xml_diff>
--- a/SettleGame.xlsx
+++ b/SettleGame.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="139">
   <si>
     <t>Conceit</t>
   </si>
@@ -271,9 +271,6 @@
     <t>Base Camp</t>
   </si>
   <si>
-    <t>Begin with three random actions from the supply of existing developments, can use developments to add additional actions</t>
-  </si>
-  <si>
     <t>Place</t>
   </si>
   <si>
@@ -434,6 +431,12 @@
   </si>
   <si>
     <t>Empty landscape of the island, islands can be created with Black developments on these</t>
+  </si>
+  <si>
+    <t>Beyond the edge of the shore, usually can't be built upon</t>
+  </si>
+  <si>
+    <t>Begin with three random active developments from the existing supply, can use effects to activate more developments</t>
   </si>
 </sst>
 </file>
@@ -961,7 +964,9 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title/>
+    <c:title>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1040,23 +1045,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="99904128"/>
-        <c:axId val="99922304"/>
+        <c:axId val="44822528"/>
+        <c:axId val="44824064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99904128"/>
+        <c:axId val="44822528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99922304"/>
+        <c:crossAx val="44824064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99922304"/>
+        <c:axId val="44824064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1064,19 +1069,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99904128"/>
+        <c:crossAx val="44822528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1118,8 +1124,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A17:G67" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A17:G67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A18:G68" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A18:G68">
     <filterColumn colId="1"/>
     <filterColumn colId="3"/>
     <filterColumn colId="4"/>
@@ -1426,10 +1432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1447,7 +1453,7 @@
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
@@ -1469,7 +1475,7 @@
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -1539,11 +1545,11 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1552,10 +1558,10 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -1564,11 +1570,11 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
@@ -1577,11 +1583,11 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -1590,11 +1596,11 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
@@ -1603,11 +1609,11 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -1615,72 +1621,66 @@
       <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="8"/>
+      <c r="A15" s="8" t="s">
+        <v>99</v>
+      </c>
       <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="C15" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="4" t="s">
+      <c r="B17" s="3"/>
+      <c r="C17" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F17" s="2" t="s">
+      <c r="E18" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="8" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -1688,7 +1688,7 @@
         <v>88</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F19" s="14" t="s">
         <v>39</v>
@@ -1699,15 +1699,15 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="8" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F20" s="14" t="s">
         <v>39</v>
@@ -1717,16 +1717,16 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>136</v>
+      <c r="A21" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>134</v>
       </c>
       <c r="F21" s="14" t="s">
         <v>39</v>
@@ -1736,16 +1736,16 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8" t="s">
-        <v>87</v>
+      <c r="A22" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16" t="s">
+        <v>96</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F22" s="14" t="s">
         <v>39</v>
@@ -1755,576 +1755,573 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F23" s="17" t="s">
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F24" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="16" t="str">
+      <c r="G24" s="16" t="str">
         <f>"+1 Food, +1 Material"</f>
         <v>+1 Food, +1 Material</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="8" t="s">
+    <row r="25" spans="1:7">
+      <c r="A25" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B25" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C25" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G24" s="8" t="str">
-        <f>"Destroy Development, +1 Action"</f>
-        <v>Destroy Development, +1 Action</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="D25" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G25" s="2" t="str">
-        <f>"-1 Treasure, +3 Actions"</f>
-        <v>-1 Treasure, +3 Actions</v>
+      <c r="G25" s="8" t="str">
+        <f>"Destroy Development, +1 Active"</f>
+        <v>Destroy Development, +1 Active</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8" t="s">
+      <c r="A26" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>78</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>136</v>
+        <v>86</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>134</v>
       </c>
       <c r="F26" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G26" s="8" t="str">
+      <c r="G26" s="2" t="str">
+        <f>"-1 Treasure, +3 Actives"</f>
+        <v>-1 Treasure, +3 Actives</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" s="8" t="str">
         <f>"-2 Treasure, build any development"</f>
         <v>-2 Treasure, build any development</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="16" t="s">
+    <row r="28" spans="1:7">
+      <c r="A28" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="F27" s="12" t="s">
+      <c r="D28" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="F28" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G27" s="16" t="str">
+      <c r="G28" s="16" t="str">
         <f xml:space="preserve"> "Destroy a Black development, +2 Material"</f>
         <v>Destroy a Black development, +2 Material</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="8" t="s">
+    <row r="29" spans="1:7">
+      <c r="A29" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8" t="s">
+      <c r="B29" s="8"/>
+      <c r="C29" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D28" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F28" s="12" t="s">
+      <c r="D29" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F29" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G28" s="8" t="str">
+      <c r="G29" s="8" t="str">
         <f>"-1 Material, For the rest of the month, all Blue developments give an additional +1 Treasure"</f>
         <v>-1 Material, For the rest of the month, all Blue developments give an additional +1 Treasure</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="2" t="s">
+    <row r="30" spans="1:7">
+      <c r="A30" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F29" s="12" t="s">
+      <c r="D30" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F30" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G29" s="2" t="str">
+      <c r="G30" s="2" t="str">
         <f>"-1 Treasure, +3 Food; or -3 Food, +1 Treasure"</f>
         <v>-1 Treasure, +3 Food; or -3 Food, +1 Treasure</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16" t="s">
+    <row r="31" spans="1:7">
+      <c r="A31" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="D30" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="F30" s="12" t="s">
+      <c r="B31" s="16"/>
+      <c r="C31" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="F31" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G30" s="16" t="str">
+      <c r="G31" s="16" t="str">
         <f>"Build a Base Camp on any Shore, destroy this Journey Pier"</f>
         <v>Build a Base Camp on any Shore, destroy this Journey Pier</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="8" t="s">
+    <row r="32" spans="1:7">
+      <c r="A32" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B32" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C32" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F31" s="12" t="s">
+      <c r="D32" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F32" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G31" s="8" t="str">
+      <c r="G32" s="8" t="str">
         <f>"-1 Treasure, +2 Treasure"</f>
         <v>-1 Treasure, +2 Treasure</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="8" t="s">
+    <row r="33" spans="1:7">
+      <c r="A33" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8" t="s">
+      <c r="B33" s="8"/>
+      <c r="C33" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F32" s="12" t="s">
+      <c r="D33" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F33" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G32" s="8" t="str">
+      <c r="G33" s="8" t="str">
         <f>"-1 Treasure, +2 Food, +2 Material"</f>
         <v>-1 Treasure, +2 Food, +2 Material</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="2" t="s">
+    <row r="34" spans="1:7">
+      <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F33" s="9" t="s">
+      <c r="D34" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F34" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G33" s="2" t="str">
+      <c r="G34" s="2" t="str">
         <f>"+1 Food"</f>
         <v>+1 Food</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16" t="s">
+    <row r="35" spans="1:7">
+      <c r="A35" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="F34" s="9" t="s">
+      <c r="D35" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="F35" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G34" s="16" t="str">
+      <c r="G35" s="16" t="str">
         <f>"For the rest of the month, Jungle, Cave, and Bog give +1 Food when used"</f>
         <v>For the rest of the month, Jungle, Cave, and Bog give +1 Food when used</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="B35" s="16"/>
-      <c r="C35" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G35" s="16" t="str">
-        <f>"Build a Jungle on Forested land, +1 Action"</f>
-        <v>Build a Jungle on Forested land, +1 Action</v>
-      </c>
-    </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E36" s="8" t="s">
+      <c r="A36" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E36" s="16" t="s">
         <v>135</v>
       </c>
       <c r="F36" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G36" s="8" t="str">
-        <f>"+1 Food, +1 Action"</f>
-        <v>+1 Food, +1 Action</v>
+      <c r="G36" s="16" t="str">
+        <f>"Build a Jungle on Forested land, +1 Active"</f>
+        <v>Build a Jungle on Forested land, +1 Active</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B37" s="8"/>
+        <v>37</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="C37" s="8" t="s">
         <v>22</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>136</v>
+        <v>88</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>134</v>
       </c>
       <c r="F37" s="9" t="s">
         <v>29</v>
       </c>
       <c r="G37" s="8" t="str">
-        <f>"Destroy 1 Pond to build this, +1 Food, +1 Material"</f>
-        <v>Destroy 1 Pond to build this, +1 Food, +1 Material</v>
+        <f>"+1 Food, +1 Active"</f>
+        <v>+1 Food, +1 Active</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="8" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8" t="s">
         <v>22</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E38" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E38" s="16" t="s">
         <v>135</v>
       </c>
       <c r="F38" s="9" t="s">
         <v>29</v>
       </c>
       <c r="G38" s="8" t="str">
-        <f>"-1 Material, +3 Food"</f>
-        <v>-1 Material, +3 Food</v>
+        <f>"Destroy 1 Pond to build this, +1 Food, +1 Material"</f>
+        <v>Destroy 1 Pond to build this, +1 Food, +1 Material</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="8" t="s">
-        <v>111</v>
+        <v>66</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D39" s="8" t="s">
-        <v>88</v>
+      <c r="D39" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F39" s="9" t="s">
         <v>29</v>
       </c>
       <c r="G39" s="8" t="str">
-        <f>"+2 Food; or +1 Food, +1 Action"</f>
-        <v>+2 Food; or +1 Food, +1 Action</v>
+        <f>"-1 Material, +3 Food"</f>
+        <v>-1 Material, +3 Food</v>
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>88</v>
+      <c r="A40" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F40" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G40" s="2" t="str">
+      <c r="G40" s="8" t="str">
+        <f>"+2 Food; or +1 Food, +1 Active"</f>
+        <v>+2 Food; or +1 Food, +1 Active</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G41" s="2" t="str">
         <f>"+2 Food"</f>
         <v>+2 Food</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="8" t="s">
+    <row r="42" spans="1:7">
+      <c r="A42" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8" t="s">
+      <c r="B42" s="8"/>
+      <c r="C42" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D42" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G42" s="8" t="str">
+        <f>"-1 Active, +1 Treasure"</f>
+        <v>-1 Active, +1 Treasure</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E41" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G41" s="8" t="str">
-        <f>"-1 Action, +1 Treasure"</f>
-        <v>-1 Action, +1 Treasure</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F42" s="10" t="s">
+      <c r="E43" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F43" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G42" s="2" t="str">
+      <c r="G43" s="2" t="str">
         <f>"+1 Material"</f>
         <v>+1 Material</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="16" t="s">
+    <row r="44" spans="1:7">
+      <c r="A44" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D43" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="E43" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="F43" s="18" t="s">
+      <c r="E44" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="F44" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="G43" s="16" t="str">
+      <c r="G44" s="16" t="str">
         <f>"Build another Rope Weaver"</f>
         <v>Build another Rope Weaver</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="B44" s="16"/>
-      <c r="C44" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="D44" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="E44" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="F44" s="18" t="s">
+    <row r="45" spans="1:7">
+      <c r="A45" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="F45" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="G44" s="16" t="str">
-        <f>"Build a Cave on Rocky land, +1 Action"</f>
-        <v>Build a Cave on Rocky land, +1 Action</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="2" t="s">
+      <c r="G45" s="16" t="str">
+        <f>"Build a Cave on Rocky land, +1 Active"</f>
+        <v>Build a Cave on Rocky land, +1 Active</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F45" s="10" t="s">
+      <c r="D46" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F46" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G45" s="2" t="str">
+      <c r="G46" s="2" t="str">
         <f>"-1 Food, +1 Treasure"</f>
         <v>-1 Food, +1 Treasure</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B46" s="8" t="s">
+    <row r="47" spans="1:7">
+      <c r="A47" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C47" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F46" s="10" t="s">
+      <c r="D47" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F47" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G46" s="8" t="str">
+      <c r="G47" s="8" t="str">
         <f>"-1 Food, +3 Material"</f>
         <v>-1 Food, +3 Material</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E47" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="F47" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G47" s="8" t="str">
-        <f>"Destroy 1 Cave to build this, +1 Treasure"</f>
-        <v>Destroy 1 Cave to build this, +1 Treasure</v>
-      </c>
-    </row>
     <row r="48" spans="1:7">
       <c r="A48" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="8" t="s">
@@ -2333,400 +2330,402 @@
       <c r="D48" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E48" s="8" t="s">
+      <c r="E48" s="16" t="s">
         <v>135</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>50</v>
       </c>
       <c r="G48" s="8" t="str">
+        <f>"Destroy 1 Cave to build this, +1 Treasure"</f>
+        <v>Destroy 1 Cave to build this, +1 Treasure</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G49" s="8" t="str">
         <f>"+2 Material"</f>
         <v>+2 Material</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="B49" s="16"/>
-      <c r="C49" s="16" t="s">
+    <row r="50" spans="1:7">
+      <c r="A50" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" s="16"/>
+      <c r="C50" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D49" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="E49" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="F49" s="18" t="s">
+      <c r="D50" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="F50" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="G49" s="16" t="str">
+      <c r="G50" s="16" t="str">
         <f>"+1 Material"</f>
         <v>+1 Material</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="8" t="s">
+    <row r="51" spans="1:7">
+      <c r="A51" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8" t="s">
+      <c r="B51" s="8"/>
+      <c r="C51" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E50" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F50" s="10" t="s">
+      <c r="D51" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F51" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G50" s="8" t="str">
+      <c r="G51" s="8" t="str">
         <f>"+1 Treasure"</f>
         <v>+1 Treasure</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
-      <c r="A51" s="8" t="s">
+    <row r="52" spans="1:7">
+      <c r="A52" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8" t="s">
+      <c r="B52" s="8"/>
+      <c r="C52" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D51" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E51" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="F51" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G51" s="8" t="str">
-        <f>"Destroy 1 Jungle to build this, +2 Actions"</f>
-        <v>Destroy 1 Jungle to build this, +2 Actions</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="D52" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E52" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E52" s="16" t="s">
         <v>135</v>
       </c>
       <c r="F52" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G52" s="2" t="str">
-        <f>"-1 Food, +2 Actions"</f>
-        <v>-1 Food, +2 Actions</v>
+      <c r="G52" s="8" t="str">
+        <f>"Destroy 1 Jungle to build this, -1 Food, +3 Actives"</f>
+        <v>Destroy 1 Jungle to build this, -1 Food, +3 Actives</v>
       </c>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8" t="s">
+      <c r="A53" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F53" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G53" s="8" t="str">
-        <f>"-1 Food, For the rest of the month, all Red developments give an additional +1 Action"</f>
-        <v>-1 Food, For the rest of the month, all Red developments give an additional +1 Action</v>
+      <c r="G53" s="2" t="str">
+        <f>"-1 Food, +2 Actives"</f>
+        <v>-1 Food, +2 Actives</v>
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="B54" s="16"/>
-      <c r="C54" s="16" t="s">
+      <c r="A54" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D54" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="E54" s="16" t="s">
-        <v>136</v>
+      <c r="D54" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>134</v>
       </c>
       <c r="F54" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G54" s="16" t="str">
-        <f>"+1 Action"</f>
-        <v>+1 Action</v>
+      <c r="G54" s="8" t="str">
+        <f>"-1 Food, For the rest of the month, all Red developments give an additional +1 Active"</f>
+        <v>-1 Food, For the rest of the month, all Red developments give an additional +1 Active</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="16" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B55" s="16"/>
       <c r="C55" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>85</v>
+        <v>21</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="E55" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F55" s="11" t="s">
         <v>30</v>
       </c>
       <c r="G55" s="16" t="str">
-        <f>"+1 Action, Perform the effect of an adjacent development"</f>
-        <v>+1 Action, Perform the effect of an adjacent development</v>
+        <f>"+1 Active"</f>
+        <v>+1 Active</v>
       </c>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>22</v>
+      <c r="A56" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16" t="s">
+        <v>105</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E56" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E56" s="16" t="s">
         <v>135</v>
       </c>
       <c r="F56" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G56" s="2" t="str">
+      <c r="G56" s="16" t="str">
+        <f>"+1 Active, Perform the effect of an adjacent development"</f>
+        <v>+1 Active, Perform the effect of an adjacent development</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F57" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G57" s="2" t="str">
         <f>"Destroy development, +1 Material"</f>
         <v>Destroy development, +1 Material</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
-      <c r="A57" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E57" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F57" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G57" s="2" t="str">
-        <f>"-1 Food, +2 Actions, +1 Material"</f>
-        <v>-1 Food, +2 Actions, +1 Material</v>
-      </c>
-    </row>
     <row r="58" spans="1:7">
       <c r="A58" s="2" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E58" s="16" t="s">
-        <v>136</v>
+        <v>84</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>134</v>
       </c>
       <c r="F58" s="11" t="s">
         <v>30</v>
       </c>
       <c r="G58" s="2" t="str">
+        <f>"-1 Food, +2 Actives, +1 Material"</f>
+        <v>-1 Food, +2 Actives, +1 Material</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E59" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G59" s="2" t="str">
         <f>"-1 Food, Destroy a non-Black development, Replace with any non-Purple development"</f>
         <v>-1 Food, Destroy a non-Black development, Replace with any non-Purple development</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
-      <c r="A59" s="8" t="s">
+    <row r="60" spans="1:7">
+      <c r="A60" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="B60" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C59" s="8" t="s">
+      <c r="C60" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D59" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E59" s="8" t="s">
+      <c r="D60" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F60" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G60" s="8" t="str">
+        <f>"-2 Food, +3 Actives"</f>
+        <v>-2 Food, +3 Actives</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B61" s="16"/>
+      <c r="C61" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F59" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G59" s="8" t="str">
-        <f>"-2 Food, +3 Actions"</f>
-        <v>-2 Food, +3 Actions</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="A60" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="B60" s="16"/>
-      <c r="C60" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="D60" s="16"/>
-      <c r="E60" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="F60" s="15" t="s">
+      <c r="F61" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="G60" s="16" t="str">
+      <c r="G61" s="16" t="str">
         <f>"Destroy 2 Black developments to build this, +1 Ship"</f>
         <v>Destroy 2 Black developments to build this, +1 Ship</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
-      <c r="A61" s="8" t="s">
+    <row r="62" spans="1:7">
+      <c r="A62" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8" t="s">
+      <c r="B62" s="8"/>
+      <c r="C62" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F61" s="15" t="s">
+      <c r="D62" s="8"/>
+      <c r="E62" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F62" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="G61" s="8" t="str">
+      <c r="G62" s="8" t="str">
         <f>"Destroy 1 Blue development to build this, +1 Ship"</f>
         <v>Destroy 1 Blue development to build this, +1 Ship</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
-      <c r="A62" s="8" t="s">
+    <row r="63" spans="1:7">
+      <c r="A63" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8" t="s">
+      <c r="B63" s="8"/>
+      <c r="C63" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F62" s="15" t="s">
+      <c r="D63" s="8"/>
+      <c r="E63" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F63" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="G62" s="8" t="str">
+      <c r="G63" s="8" t="str">
         <f>"Destroy 1 Green development to build this, +1 Ship"</f>
         <v>Destroy 1 Green development to build this, +1 Ship</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="8" t="s">
+    <row r="64" spans="1:7">
+      <c r="A64" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B63" s="8"/>
-      <c r="C63" s="8" t="s">
+      <c r="B64" s="8"/>
+      <c r="C64" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D63" s="8"/>
-      <c r="E63" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="F63" s="15" t="s">
+      <c r="D64" s="8"/>
+      <c r="E64" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="F64" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="G63" s="8" t="str">
+      <c r="G64" s="8" t="str">
         <f>"Destroy 1 Red development to build this, +2 Ships"</f>
         <v>Destroy 1 Red development to build this, +2 Ships</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
-      <c r="A64" s="8" t="s">
+    <row r="65" spans="1:7">
+      <c r="A65" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B64" s="8"/>
-      <c r="C64" s="8" t="s">
+      <c r="B65" s="8"/>
+      <c r="C65" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F64" s="15" t="s">
+      <c r="D65" s="8"/>
+      <c r="E65" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F65" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="G64" s="8" t="str">
+      <c r="G65" s="8" t="str">
         <f>"Destroy 1 Orange development to build this, +1 Ship"</f>
         <v>Destroy 1 Orange development to build this, +1 Ship</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
-      <c r="A65" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B65" s="8"/>
-      <c r="C65" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F65" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="G65" s="8" t="str">
-        <f>"+1 Ship"</f>
-        <v>+1 Ship</v>
-      </c>
-    </row>
     <row r="66" spans="1:7">
       <c r="A66" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B66" s="8"/>
       <c r="C66" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D66" s="8"/>
       <c r="E66" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F66" s="15" t="s">
         <v>64</v>
@@ -2738,20 +2737,40 @@
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B67" s="8"/>
       <c r="C67" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D67" s="8"/>
       <c r="E67" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F67" s="15" t="s">
         <v>64</v>
       </c>
       <c r="G67" s="8" t="str">
+        <f>"+1 Ship"</f>
+        <v>+1 Ship</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F68" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G68" s="8" t="str">
         <f>"+1 Ship"</f>
         <v>+1 Ship</v>
       </c>
@@ -2769,7 +2788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
@@ -4365,14 +4384,14 @@
       </c>
       <c r="O33" s="34"/>
       <c r="R33" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="10:18" ht="30" customHeight="1">
       <c r="J34" s="32"/>
       <c r="O34" s="26"/>
       <c r="R34" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="10:18" ht="30" customHeight="1">
@@ -4391,7 +4410,7 @@
       </c>
       <c r="O35" s="28"/>
       <c r="R35" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="10:18" ht="30" customHeight="1">
@@ -4414,7 +4433,7 @@
         <v>8</v>
       </c>
       <c r="R36" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="10:18" ht="30" customHeight="1">
@@ -4455,7 +4474,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B1">
         <v>3</v>
@@ -4463,7 +4482,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B2">
         <v>1.5</v>
@@ -4471,15 +4490,15 @@
     </row>
     <row r="4" spans="1:3">
       <c r="B4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" t="s">
         <v>128</v>
-      </c>
-      <c r="C4" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B5">
         <f>0.5*width</f>
@@ -4491,7 +4510,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B6">
         <f>(0.5*width-0.5*height)</f>
@@ -4504,7 +4523,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B7">
         <f>-(0.5*width-0.5*height)</f>
@@ -4517,7 +4536,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B8">
         <v>-1.5</v>
@@ -4528,7 +4547,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B9">
         <f>-(0.5*width-0.5*height)</f>
@@ -4541,7 +4560,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B10">
         <f>(0.5*width-0.5*height)</f>

</xml_diff>

<commit_message>
Add parentID with hex class to link tiles with lands  Changes to be committed: 	modified:   SettleGame.xlsx 	modified:   app/__init__.pyc 	modified:   app/static/js/main.ts
</commit_message>
<xml_diff>
--- a/SettleGame.xlsx
+++ b/SettleGame.xlsx
@@ -15,12 +15,12 @@
     <definedName name="height">Hexagons!$B$2</definedName>
     <definedName name="width">Hexagons!$B$1</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="140">
   <si>
     <t>Conceit</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Material</t>
   </si>
   <si>
-    <t>Used to develop</t>
-  </si>
-  <si>
     <t>Used to feed people/animals</t>
   </si>
   <si>
@@ -136,9 +133,6 @@
     <t>Hunting Camp</t>
   </si>
   <si>
-    <t>Zebu Ranch</t>
-  </si>
-  <si>
     <t>Black</t>
   </si>
   <si>
@@ -301,9 +295,6 @@
     <t>Faces the sea, the initial Base Camp must be built here, Blue developments are built here</t>
   </si>
   <si>
-    <t>Covered with bamboo or arboreal forest, some Blue or Orange developments built here</t>
-  </si>
-  <si>
     <t>Good for growing, the dominant type in most islands, many Green developments are built here</t>
   </si>
   <si>
@@ -358,18 +349,12 @@
     <t>Strategically develop an island to survive the rainy season or compete with other players</t>
   </si>
   <si>
-    <t>Pond</t>
-  </si>
-  <si>
     <t>Raft Village</t>
   </si>
   <si>
     <t>Ruins</t>
   </si>
   <si>
-    <t>Explorer</t>
-  </si>
-  <si>
     <t>1T</t>
   </si>
   <si>
@@ -430,13 +415,31 @@
     <t>Journey</t>
   </si>
   <si>
-    <t>Empty landscape of the island, islands can be created with Black developments on these</t>
-  </si>
-  <si>
     <t>Beyond the edge of the shore, usually can't be built upon</t>
   </si>
   <si>
     <t>Begin with three random active developments from the existing supply, can use effects to activate more developments</t>
+  </si>
+  <si>
+    <t>Used to build developments</t>
+  </si>
+  <si>
+    <t>Empty landscape of the island, developments can only be built on certain landscapes</t>
+  </si>
+  <si>
+    <t>Freshwater</t>
+  </si>
+  <si>
+    <t>Covered with bamboo or arboreal forest, some Green or Orange developments built here</t>
+  </si>
+  <si>
+    <t>Boar Ranch</t>
+  </si>
+  <si>
+    <t>Poacher's Dock</t>
+  </si>
+  <si>
+    <t>Explorer's Quarters</t>
   </si>
 </sst>
 </file>
@@ -1045,23 +1048,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="44822528"/>
-        <c:axId val="44824064"/>
+        <c:axId val="94792704"/>
+        <c:axId val="121558912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44822528"/>
+        <c:axId val="94792704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44824064"/>
+        <c:crossAx val="121558912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44824064"/>
+        <c:axId val="121558912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1069,7 +1072,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44822528"/>
+        <c:crossAx val="94792704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1082,7 +1085,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1124,15 +1127,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A18:G68" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A18:G68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A18:G69" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A18:G69">
     <filterColumn colId="1"/>
     <filterColumn colId="3"/>
     <filterColumn colId="4"/>
     <filterColumn colId="5"/>
   </autoFilter>
-  <sortState ref="A18:G67">
-    <sortCondition ref="F17:F67"/>
+  <sortState ref="A19:G69">
+    <sortCondition ref="F18:F69"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" name="Name" dataDxfId="6"/>
@@ -1432,16 +1435,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14" hidden="1" customWidth="1"/>
     <col min="3" max="4" width="10.140625" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="99.140625" customWidth="1"/>
@@ -1453,7 +1456,7 @@
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
@@ -1475,7 +1478,7 @@
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -1488,7 +1491,7 @@
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8" t="s">
-        <v>3</v>
+        <v>133</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
@@ -1497,11 +1500,11 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -1510,11 +1513,11 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -1523,11 +1526,11 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -1545,11 +1548,11 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1558,10 +1561,10 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -1570,11 +1573,11 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
@@ -1583,11 +1586,11 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8" t="s">
-        <v>93</v>
+        <v>136</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -1596,11 +1599,11 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
@@ -1609,11 +1612,11 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -1622,11 +1625,11 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -1644,11 +1647,11 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="4" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1657,136 +1660,136 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="8" t="s">
-        <v>112</v>
+        <v>135</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="16" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G24" s="16" t="str">
         <f>"+1 Food, +1 Material"</f>
@@ -1795,22 +1798,22 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G25" s="8" t="str">
         <f>"Destroy Development, +1 Active"</f>
@@ -1819,22 +1822,22 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G26" s="2" t="str">
         <f>"-1 Treasure, +3 Actives"</f>
@@ -1843,20 +1846,20 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G27" s="8" t="str">
         <f>"-2 Treasure, build any development"</f>
@@ -1865,20 +1868,20 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="16" t="s">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="16" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G28" s="16" t="str">
         <f xml:space="preserve"> "Destroy a Black development, +2 Material"</f>
@@ -1886,869 +1889,871 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8" t="s">
-        <v>71</v>
+      <c r="A29" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16" t="s">
+        <v>111</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>134</v>
+        <v>84</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G29" s="8" t="str">
+        <v>30</v>
+      </c>
+      <c r="G29" s="16" t="str">
+        <f xml:space="preserve"> "Destroy a Black development, +2 Food"</f>
+        <v>Destroy a Black development, +2 Food</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" s="8" t="str">
         <f>"-1 Material, For the rest of the month, all Blue developments give an additional +1 Treasure"</f>
         <v>-1 Material, For the rest of the month, all Blue developments give an additional +1 Treasure</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G30" s="2" t="str">
+    <row r="31" spans="1:7">
+      <c r="A31" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G31" s="2" t="str">
         <f>"-1 Treasure, +3 Food; or -3 Food, +1 Treasure"</f>
         <v>-1 Treasure, +3 Food; or -3 Food, +1 Treasure</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G31" s="16" t="str">
+    <row r="32" spans="1:7">
+      <c r="A32" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" s="16" t="str">
         <f>"Build a Base Camp on any Shore, destroy this Journey Pier"</f>
         <v>Build a Base Camp on any Shore, destroy this Journey Pier</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="8" t="s">
+    <row r="33" spans="1:7">
+      <c r="A33" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G32" s="8" t="str">
+      <c r="D33" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G33" s="8" t="str">
         <f>"-1 Treasure, +2 Treasure"</f>
         <v>-1 Treasure, +2 Treasure</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G33" s="8" t="str">
+    <row r="34" spans="1:7">
+      <c r="A34" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G34" s="8" t="str">
         <f>"-1 Treasure, +2 Food, +2 Material"</f>
         <v>-1 Treasure, +2 Food, +2 Material</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G34" s="2" t="str">
+    <row r="35" spans="1:7">
+      <c r="A35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G35" s="2" t="str">
         <f>"+1 Food"</f>
         <v>+1 Food</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="B35" s="16"/>
-      <c r="C35" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G35" s="16" t="str">
+    <row r="36" spans="1:7">
+      <c r="A36" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" s="16" t="str">
         <f>"For the rest of the month, Jungle, Cave, and Bog give +1 Food when used"</f>
         <v>For the rest of the month, Jungle, Cave, and Bog give +1 Food when used</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G36" s="16" t="str">
+    <row r="37" spans="1:7">
+      <c r="A37" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G37" s="16" t="str">
         <f>"Build a Jungle on Forested land, +1 Active"</f>
         <v>Build a Jungle on Forested land, +1 Active</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G37" s="8" t="str">
+    <row r="38" spans="1:7">
+      <c r="A38" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G38" s="8" t="str">
         <f>"+1 Food, +1 Active"</f>
         <v>+1 Food, +1 Active</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G38" s="8" t="str">
-        <f>"Destroy 1 Pond to build this, +1 Food, +1 Material"</f>
-        <v>Destroy 1 Pond to build this, +1 Food, +1 Material</v>
-      </c>
-    </row>
     <row r="39" spans="1:7">
       <c r="A39" s="8" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E39" s="8" t="s">
-        <v>134</v>
+      <c r="E39" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G39" s="8" t="str">
+        <f>"Destroy 1 Freshwater to build this, +1 Food, +1 Material"</f>
+        <v>Destroy 1 Freshwater to build this, +1 Food, +1 Material</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40" s="8" t="str">
         <f>"-1 Material, +3 Food"</f>
         <v>-1 Material, +3 Food</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8" t="s">
+    <row r="41" spans="1:7">
+      <c r="A41" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G41" s="8" t="str">
+        <f>"+2 Food; or +1 Active"</f>
+        <v>+2 Food; or +1 Active</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D40" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G40" s="8" t="str">
-        <f>"+2 Food; or +1 Food, +1 Active"</f>
-        <v>+2 Food; or +1 Food, +1 Active</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G41" s="2" t="str">
-        <f>"+2 Food"</f>
-        <v>+2 Food</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8" t="s">
-        <v>57</v>
-      </c>
       <c r="D42" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E42" s="16" t="s">
-        <v>135</v>
+        <v>85</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>129</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G42" s="8" t="str">
+        <v>28</v>
+      </c>
+      <c r="G42" s="2" t="str">
+        <f>"-1 Food, +3 Food"</f>
+        <v>-1 Food, +3 Food</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" s="8" t="str">
         <f>"-1 Active, +1 Treasure"</f>
         <v>-1 Active, +1 Treasure</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G43" s="2" t="str">
+    <row r="44" spans="1:7">
+      <c r="A44" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G44" s="2" t="str">
         <f>"+1 Material"</f>
         <v>+1 Material</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="B44" s="16"/>
-      <c r="C44" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D44" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="E44" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="F44" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G44" s="16" t="str">
+    <row r="45" spans="1:7">
+      <c r="A45" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G45" s="16" t="str">
         <f>"Build another Rope Weaver"</f>
         <v>Build another Rope Weaver</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="B45" s="16"/>
-      <c r="C45" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="D45" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="E45" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="F45" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G45" s="16" t="str">
+    <row r="46" spans="1:7">
+      <c r="A46" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="F46" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G46" s="16" t="str">
         <f>"Build a Cave on Rocky land, +1 Active"</f>
         <v>Build a Cave on Rocky land, +1 Active</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F46" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G46" s="2" t="str">
+    <row r="47" spans="1:7">
+      <c r="A47" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G47" s="2" t="str">
         <f>"-1 Food, +1 Treasure"</f>
         <v>-1 Food, +1 Treasure</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F47" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G47" s="8" t="str">
+    <row r="48" spans="1:7">
+      <c r="A48" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G48" s="8" t="str">
         <f>"-1 Food, +3 Material"</f>
         <v>-1 Food, +3 Material</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E48" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="F48" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G48" s="8" t="str">
+    <row r="49" spans="1:7">
+      <c r="A49" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G49" s="8" t="str">
         <f>"Destroy 1 Cave to build this, +1 Treasure"</f>
         <v>Destroy 1 Cave to build this, +1 Treasure</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E49" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F49" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G49" s="8" t="str">
+    <row r="50" spans="1:7">
+      <c r="A50" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G50" s="8" t="str">
         <f>"+2 Material"</f>
         <v>+2 Material</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="B50" s="16"/>
-      <c r="C50" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="E50" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="F50" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G50" s="16" t="str">
+    <row r="51" spans="1:7">
+      <c r="A51" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" s="16"/>
+      <c r="C51" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="F51" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G51" s="16" t="str">
         <f>"+1 Material"</f>
         <v>+1 Material</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
-      <c r="A51" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F51" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G51" s="8" t="str">
+    <row r="52" spans="1:7">
+      <c r="A52" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G52" s="8" t="str">
         <f>"+1 Treasure"</f>
         <v>+1 Treasure</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
-      <c r="A52" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E52" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="F52" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G52" s="8" t="str">
+    <row r="53" spans="1:7">
+      <c r="A53" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E53" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="F53" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G53" s="8" t="str">
         <f>"Destroy 1 Jungle to build this, -1 Food, +3 Actives"</f>
         <v>Destroy 1 Jungle to build this, -1 Food, +3 Actives</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
-      <c r="A53" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F53" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G53" s="2" t="str">
+    <row r="54" spans="1:7">
+      <c r="A54" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G54" s="2" t="str">
         <f>"-1 Food, +2 Actives"</f>
         <v>-1 Food, +2 Actives</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
-      <c r="A54" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F54" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G54" s="8" t="str">
+    <row r="55" spans="1:7">
+      <c r="A55" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F55" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G55" s="8" t="str">
         <f>"-1 Food, For the rest of the month, all Red developments give an additional +1 Active"</f>
         <v>-1 Food, For the rest of the month, all Red developments give an additional +1 Active</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
-      <c r="A55" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="B55" s="16"/>
-      <c r="C55" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D55" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="E55" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="F55" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G55" s="16" t="str">
+    <row r="56" spans="1:7">
+      <c r="A56" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="E56" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G56" s="16" t="str">
         <f>"+1 Active"</f>
         <v>+1 Active</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
-      <c r="A56" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="B56" s="16"/>
-      <c r="C56" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E56" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="F56" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G56" s="16" t="str">
+    <row r="57" spans="1:7">
+      <c r="A57" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B57" s="16"/>
+      <c r="C57" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E57" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="F57" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G57" s="16" t="str">
         <f>"+1 Active, Perform the effect of an adjacent development"</f>
         <v>+1 Active, Perform the effect of an adjacent development</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
-      <c r="A57" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E57" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F57" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G57" s="2" t="str">
+    <row r="58" spans="1:7">
+      <c r="A58" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G58" s="2" t="str">
         <f>"Destroy development, +1 Material"</f>
         <v>Destroy development, +1 Material</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
-      <c r="A58" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E58" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F58" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G58" s="2" t="str">
+    <row r="59" spans="1:7">
+      <c r="A59" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G59" s="2" t="str">
         <f>"-1 Food, +2 Actives, +1 Material"</f>
         <v>-1 Food, +2 Actives, +1 Material</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
-      <c r="A59" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E59" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="F59" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G59" s="2" t="str">
-        <f>"-1 Food, Destroy a non-Black development, Replace with any non-Purple development"</f>
-        <v>-1 Food, Destroy a non-Black development, Replace with any non-Purple development</v>
-      </c>
-    </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>25</v>
+      <c r="A60" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>134</v>
+        <v>82</v>
+      </c>
+      <c r="E60" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G60" s="8" t="str">
+        <v>29</v>
+      </c>
+      <c r="G60" s="2" t="str">
+        <f>"-1 Food, Destroy a non-Black development, Replace with any non-Violet development"</f>
+        <v>-1 Food, Destroy a non-Black development, Replace with any non-Violet development</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F61" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G61" s="8" t="str">
         <f>"-2 Food, +3 Actives"</f>
         <v>-2 Food, +3 Actives</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
-      <c r="A61" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="B61" s="16"/>
-      <c r="C61" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="D61" s="16"/>
-      <c r="E61" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="F61" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="G61" s="16" t="str">
+    <row r="62" spans="1:7">
+      <c r="A62" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B62" s="16"/>
+      <c r="C62" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="F62" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G62" s="16" t="str">
         <f>"Destroy 2 Black developments to build this, +1 Ship"</f>
         <v>Destroy 2 Black developments to build this, +1 Ship</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
-      <c r="A62" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F62" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="G62" s="8" t="str">
+    <row r="63" spans="1:7">
+      <c r="A63" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F63" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G63" s="8" t="str">
         <f>"Destroy 1 Blue development to build this, +1 Ship"</f>
         <v>Destroy 1 Blue development to build this, +1 Ship</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B63" s="8"/>
-      <c r="C63" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F63" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="G63" s="8" t="str">
+    <row r="64" spans="1:7">
+      <c r="A64" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F64" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G64" s="8" t="str">
         <f>"Destroy 1 Green development to build this, +1 Ship"</f>
         <v>Destroy 1 Green development to build this, +1 Ship</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
-      <c r="A64" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B64" s="8"/>
-      <c r="C64" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D64" s="8"/>
-      <c r="E64" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="F64" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="G64" s="8" t="str">
+    <row r="65" spans="1:7">
+      <c r="A65" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B65" s="8"/>
+      <c r="C65" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D65" s="8"/>
+      <c r="E65" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="F65" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G65" s="8" t="str">
         <f>"Destroy 1 Red development to build this, +2 Ships"</f>
         <v>Destroy 1 Red development to build this, +2 Ships</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
-      <c r="A65" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B65" s="8"/>
-      <c r="C65" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F65" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="G65" s="8" t="str">
+    <row r="66" spans="1:7">
+      <c r="A66" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B66" s="8"/>
+      <c r="C66" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F66" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G66" s="8" t="str">
         <f>"Destroy 1 Orange development to build this, +1 Ship"</f>
         <v>Destroy 1 Orange development to build this, +1 Ship</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
-      <c r="A66" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B66" s="8"/>
-      <c r="C66" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D66" s="8"/>
-      <c r="E66" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="F66" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="G66" s="8" t="str">
-        <f>"+1 Ship"</f>
-        <v>+1 Ship</v>
-      </c>
-    </row>
     <row r="67" spans="1:7">
       <c r="A67" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B67" s="8"/>
       <c r="C67" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D67" s="8"/>
       <c r="E67" s="8" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F67" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G67" s="8" t="str">
         <f>"+1 Ship"</f>
@@ -2757,20 +2762,40 @@
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B68" s="8"/>
       <c r="C68" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D68" s="8"/>
       <c r="E68" s="8" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F68" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G68" s="8" t="str">
+        <f>"+1 Ship"</f>
+        <v>+1 Ship</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B69" s="8"/>
+      <c r="C69" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F69" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G69" s="8" t="str">
         <f>"+1 Ship"</f>
         <v>+1 Ship</v>
       </c>
@@ -4384,14 +4409,14 @@
       </c>
       <c r="O33" s="34"/>
       <c r="R33" s="19" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="10:18" ht="30" customHeight="1">
       <c r="J34" s="32"/>
       <c r="O34" s="26"/>
       <c r="R34" s="19" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="10:18" ht="30" customHeight="1">
@@ -4410,7 +4435,7 @@
       </c>
       <c r="O35" s="28"/>
       <c r="R35" s="19" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="10:18" ht="30" customHeight="1">
@@ -4433,7 +4458,7 @@
         <v>8</v>
       </c>
       <c r="R36" s="19" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="10:18" ht="30" customHeight="1">
@@ -4474,7 +4499,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B1">
         <v>3</v>
@@ -4482,7 +4507,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B2">
         <v>1.5</v>
@@ -4490,15 +4515,15 @@
     </row>
     <row r="4" spans="1:3">
       <c r="B4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B5">
         <f>0.5*width</f>
@@ -4510,7 +4535,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B6">
         <f>(0.5*width-0.5*height)</f>
@@ -4523,7 +4548,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B7">
         <f>-(0.5*width-0.5*height)</f>
@@ -4536,7 +4561,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B8">
         <v>-1.5</v>
@@ -4547,7 +4572,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B9">
         <f>-(0.5*width-0.5*height)</f>
@@ -4560,7 +4585,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B10">
         <f>(0.5*width-0.5*height)</f>

</xml_diff>

<commit_message>
Development and landscape classes
 Changes to be committed:
	modified:   SettleGame.xlsx
	modified:   app/static/js/main.js
	modified:   app/static/js/main.ts
</commit_message>
<xml_diff>
--- a/SettleGame.xlsx
+++ b/SettleGame.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="17925" windowHeight="6645"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="1" r:id="rId1"/>
     <sheet name="Mapping" sheetId="2" r:id="rId2"/>
     <sheet name="Hexagons" sheetId="3" r:id="rId3"/>
+    <sheet name="RandGen" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="height">Hexagons!$B$2</definedName>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="146">
   <si>
     <t>Conceit</t>
   </si>
@@ -440,13 +441,31 @@
   </si>
   <si>
     <t>Explorer's Quarters</t>
+  </si>
+  <si>
+    <t>Random land generation process</t>
+  </si>
+  <si>
+    <t>Beginning structure consists of grass and sea</t>
+  </si>
+  <si>
+    <t>Shape and size of this defined by user input</t>
+  </si>
+  <si>
+    <t>Beginning from the center, grass is changed randomly to the other types, excepting sea</t>
+  </si>
+  <si>
+    <t>This process repeats at least twice, with similar tiles being more likely to be created next to one another</t>
+  </si>
+  <si>
+    <t>On the final pass, shore is created on any tile bordering sea</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,6 +507,14 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -753,7 +780,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -815,6 +842,15 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1048,23 +1084,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="94792704"/>
-        <c:axId val="121558912"/>
+        <c:axId val="109482752"/>
+        <c:axId val="109484288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94792704"/>
+        <c:axId val="109482752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121558912"/>
+        <c:crossAx val="109484288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121558912"/>
+        <c:axId val="109484288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1072,7 +1108,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94792704"/>
+        <c:crossAx val="109482752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1085,7 +1121,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1131,7 +1167,11 @@
   <autoFilter ref="A18:G69">
     <filterColumn colId="1"/>
     <filterColumn colId="3"/>
-    <filterColumn colId="4"/>
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Basic"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="5"/>
   </autoFilter>
   <sortState ref="A19:G69">
@@ -1437,8 +1477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1738,7 +1778,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" hidden="1">
       <c r="A22" s="16" t="s">
         <v>110</v>
       </c>
@@ -1757,7 +1797,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" hidden="1">
       <c r="A23" s="8" t="s">
         <v>68</v>
       </c>
@@ -1844,7 +1884,7 @@
         <v>-1 Treasure, +3 Actives</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" hidden="1">
       <c r="A27" s="8" t="s">
         <v>75</v>
       </c>
@@ -1866,7 +1906,7 @@
         <v>-2 Treasure, build any development</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" hidden="1">
       <c r="A28" s="16" t="s">
         <v>139</v>
       </c>
@@ -1888,7 +1928,7 @@
         <v>Destroy a Black development, +2 Material</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" hidden="1">
       <c r="A29" s="16" t="s">
         <v>138</v>
       </c>
@@ -1956,7 +1996,7 @@
         <v>-1 Treasure, +3 Food; or -3 Food, +1 Treasure</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" hidden="1">
       <c r="A32" s="16" t="s">
         <v>99</v>
       </c>
@@ -2048,7 +2088,7 @@
         <v>+1 Food</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" hidden="1">
       <c r="A36" s="16" t="s">
         <v>97</v>
       </c>
@@ -2070,7 +2110,7 @@
         <v>For the rest of the month, Jungle, Cave, and Bog give +1 Food when used</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" hidden="1">
       <c r="A37" s="16" t="s">
         <v>112</v>
       </c>
@@ -2116,7 +2156,7 @@
         <v>+1 Food, +1 Active</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" hidden="1">
       <c r="A39" s="8" t="s">
         <v>49</v>
       </c>
@@ -2206,7 +2246,7 @@
         <v>-1 Food, +3 Food</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" hidden="1">
       <c r="A43" s="8" t="s">
         <v>71</v>
       </c>
@@ -2252,7 +2292,7 @@
         <v>+1 Material</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" hidden="1">
       <c r="A45" s="16" t="s">
         <v>95</v>
       </c>
@@ -2274,7 +2314,7 @@
         <v>Build another Rope Weaver</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" hidden="1">
       <c r="A46" s="16" t="s">
         <v>113</v>
       </c>
@@ -2344,7 +2384,7 @@
         <v>-1 Food, +3 Material</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" hidden="1">
       <c r="A49" s="8" t="s">
         <v>42</v>
       </c>
@@ -2388,7 +2428,7 @@
         <v>+2 Material</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" hidden="1">
       <c r="A51" s="16" t="s">
         <v>100</v>
       </c>
@@ -2432,7 +2472,7 @@
         <v>+1 Treasure</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" hidden="1">
       <c r="A53" s="8" t="s">
         <v>40</v>
       </c>
@@ -2500,7 +2540,7 @@
         <v>-1 Food, For the rest of the month, all Red developments give an additional +1 Active</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" hidden="1">
       <c r="A56" s="16" t="s">
         <v>109</v>
       </c>
@@ -2522,7 +2562,7 @@
         <v>+1 Active</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" hidden="1">
       <c r="A57" s="16" t="s">
         <v>101</v>
       </c>
@@ -2592,7 +2632,7 @@
         <v>-1 Food, +2 Actives, +1 Material</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" hidden="1">
       <c r="A60" s="2" t="s">
         <v>19</v>
       </c>
@@ -2640,7 +2680,7 @@
         <v>-2 Food, +3 Actives</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" hidden="1">
       <c r="A62" s="16" t="s">
         <v>104</v>
       </c>
@@ -2700,7 +2740,7 @@
         <v>Destroy 1 Green development to build this, +1 Ship</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" hidden="1">
       <c r="A65" s="8" t="s">
         <v>50</v>
       </c>
@@ -2814,7 +2854,7 @@
   <dimension ref="A1:AE38"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="30" customHeight="1"/>
@@ -4600,4 +4640,74 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3.42578125" style="45" customWidth="1"/>
+    <col min="2" max="2" width="44" style="46" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="45"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="44"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="45">
+        <v>1</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="45">
+        <v>2</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30">
+      <c r="A4" s="45">
+        <v>3</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="45">
+      <c r="A5" s="45">
+        <v>4</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30">
+      <c r="A6" s="45">
+        <v>5</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Game design typo/ordering fixes
 Changes to be committed:
	modified:   SettleGame.xlsx
	modified:   app/static/js/main.ts
</commit_message>
<xml_diff>
--- a/SettleGame.xlsx
+++ b/SettleGame.xlsx
@@ -1477,8 +1477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1992,8 +1992,8 @@
         <v>30</v>
       </c>
       <c r="G31" s="2" t="str">
-        <f>"-1 Treasure, +3 Food; or -3 Food, +1 Treasure"</f>
-        <v>-1 Treasure, +3 Food; or -3 Food, +1 Treasure</v>
+        <f>"-1 Food, -1 Material, +1 Treasure"</f>
+        <v>-1 Food, -1 Material, +1 Treasure</v>
       </c>
     </row>
     <row r="32" spans="1:7" hidden="1">
@@ -2133,17 +2133,17 @@
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>21</v>
+      <c r="A38" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>129</v>
@@ -2151,64 +2151,66 @@
       <c r="F38" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G38" s="8" t="str">
+      <c r="G38" s="2" t="str">
+        <f>"-1 Food, +3 Food"</f>
+        <v>-1 Food, +3 Food</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39" s="8" t="str">
         <f>"+1 Food, +1 Active"</f>
         <v>+1 Food, +1 Active</v>
       </c>
     </row>
-    <row r="39" spans="1:7" hidden="1">
-      <c r="A39" s="8" t="s">
+    <row r="40" spans="1:7" hidden="1">
+      <c r="A40" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="F39" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G39" s="8" t="str">
-        <f>"Destroy 1 Freshwater to build this, +1 Food, +1 Material"</f>
-        <v>Destroy 1 Freshwater to build this, +1 Food, +1 Material</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="8" t="s">
-        <v>64</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>129</v>
+        <v>87</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="F40" s="9" t="s">
         <v>28</v>
       </c>
       <c r="G40" s="8" t="str">
-        <f>"-1 Material, +3 Food"</f>
-        <v>-1 Material, +3 Food</v>
+        <f>"Destroy 1 Freshwater to build this, +1 Food, +1 Material"</f>
+        <v>Destroy 1 Freshwater to build this, +1 Food, +1 Material</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="8" t="s">
-        <v>107</v>
+        <v>64</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="2" t="s">
         <v>85</v>
       </c>
       <c r="E41" s="8" t="s">
@@ -2218,21 +2220,19 @@
         <v>28</v>
       </c>
       <c r="G41" s="8" t="str">
-        <f>"+2 Food; or +1 Active"</f>
-        <v>+2 Food; or +1 Active</v>
+        <f>"-1 Material, +3 Food"</f>
+        <v>-1 Material, +3 Food</v>
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D42" s="2" t="s">
+      <c r="A42" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" s="8" t="s">
         <v>85</v>
       </c>
       <c r="E42" s="8" t="s">
@@ -2241,9 +2241,9 @@
       <c r="F42" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G42" s="2" t="str">
-        <f>"-1 Food, +3 Food"</f>
-        <v>-1 Food, +3 Food</v>
+      <c r="G42" s="8" t="str">
+        <f>"+2 Food"</f>
+        <v>+2 Food</v>
       </c>
     </row>
     <row r="43" spans="1:7" hidden="1">
@@ -2356,8 +2356,8 @@
         <v>48</v>
       </c>
       <c r="G47" s="2" t="str">
-        <f>"-1 Food, +1 Treasure"</f>
-        <v>-1 Food, +1 Treasure</v>
+        <f>"-2 Food, +1 Treasure"</f>
+        <v>-2 Food, +1 Treasure</v>
       </c>
     </row>
     <row r="48" spans="1:7">

</xml_diff>

<commit_message>
Incomplete random land generation
 Changes to be committed:
	modified:   SettleGame.xlsx
	modified:   app/static/js/main.ts
</commit_message>
<xml_diff>
--- a/SettleGame.xlsx
+++ b/SettleGame.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="17925" windowHeight="6645"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="17925" windowHeight="6645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="151">
   <si>
     <t>Conceit</t>
   </si>
@@ -452,13 +452,28 @@
     <t>Shape and size of this defined by user input</t>
   </si>
   <si>
-    <t>Beginning from the center, grass is changed randomly to the other types, excepting sea</t>
-  </si>
-  <si>
     <t>This process repeats at least twice, with similar tiles being more likely to be created next to one another</t>
   </si>
   <si>
     <t>On the final pass, shore is created on any tile bordering sea</t>
+  </si>
+  <si>
+    <t>Beginning from the center, grass is changed randomly to the other types</t>
+  </si>
+  <si>
+    <t>An array is made reflecting all the neighboring landscape types</t>
+  </si>
+  <si>
+    <t>This array is adjusted so that it adds up to a maximum of 0.5</t>
+  </si>
+  <si>
+    <t>This array is multiplied by the landscape's climate array</t>
+  </si>
+  <si>
+    <t>If a non-sea tile borders the sea, there is a n/6/2 chance that it will be changed into a sea tile.</t>
+  </si>
+  <si>
+    <t>If a sea tile borders the land, there is a n/6/2 chance that it will be changed into a non-sea tile.</t>
   </si>
 </sst>
 </file>
@@ -843,14 +858,14 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1003,9 +1018,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1084,23 +1097,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="109482752"/>
-        <c:axId val="109484288"/>
+        <c:axId val="111674112"/>
+        <c:axId val="111675648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109482752"/>
+        <c:axId val="111674112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109484288"/>
+        <c:crossAx val="111675648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109484288"/>
+        <c:axId val="111675648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1108,20 +1121,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109482752"/>
+        <c:crossAx val="111674112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1477,7 +1489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
@@ -4644,63 +4656,103 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" style="45" customWidth="1"/>
-    <col min="2" max="2" width="44" style="46" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="45"/>
+    <col min="1" max="1" width="4" style="44" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44" style="45" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="44"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="44"/>
+      <c r="B1" s="46"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="45">
+      <c r="A2" s="44">
         <v>1</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="45" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="45">
+      <c r="A3" s="44">
         <v>2</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="45" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30">
-      <c r="A4" s="45">
+      <c r="A4" s="44">
         <v>3</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="45" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30">
+      <c r="A5" s="44">
+        <v>3.1</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30">
+      <c r="A6" s="44">
+        <v>3.2</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30">
+      <c r="A7" s="44">
+        <v>3.3</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="45">
+      <c r="A8" s="44">
+        <v>3.4</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="45">
+      <c r="A9" s="44">
+        <v>3.5</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="45">
+      <c r="A10" s="44">
+        <v>4</v>
+      </c>
+      <c r="B10" s="45" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="45">
-      <c r="A5" s="45">
-        <v>4</v>
-      </c>
-      <c r="B5" s="46" t="s">
+    <row r="11" spans="1:2" ht="30">
+      <c r="A11" s="44">
+        <v>5</v>
+      </c>
+      <c r="B11" s="45" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="30">
-      <c r="A6" s="45">
-        <v>5</v>
-      </c>
-      <c r="B6" s="46" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added all basic developments
</commit_message>
<xml_diff>
--- a/SettleGame.xlsx
+++ b/SettleGame.xlsx
@@ -230,9 +230,6 @@
     <t>2F, 2M, 2T</t>
   </si>
   <si>
-    <t>Horseman Village</t>
-  </si>
-  <si>
     <t>Spice Farm</t>
   </si>
   <si>
@@ -471,6 +468,9 @@
   </si>
   <si>
     <t>If a sea tile borders the land, there is a n/6/2 chance that it will be changed into a non-sea tile.</t>
+  </si>
+  <si>
+    <t>Shepherd Village</t>
   </si>
 </sst>
 </file>
@@ -1122,23 +1122,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="37594624"/>
-        <c:axId val="37596160"/>
+        <c:axId val="80375168"/>
+        <c:axId val="80630912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="37594624"/>
+        <c:axId val="80375168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37596160"/>
+        <c:crossAx val="80630912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="37596160"/>
+        <c:axId val="80630912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1146,7 +1146,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37594624"/>
+        <c:crossAx val="80375168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1158,7 +1158,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1514,8 +1514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1533,7 +1533,7 @@
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
@@ -1555,7 +1555,7 @@
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -1568,7 +1568,7 @@
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
@@ -1625,11 +1625,11 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1638,10 +1638,10 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -1650,11 +1650,11 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
@@ -1663,11 +1663,11 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -1676,11 +1676,11 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
@@ -1689,11 +1689,11 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -1702,11 +1702,11 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1746,10 +1746,10 @@
         <v>9</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>27</v>
@@ -1760,15 +1760,15 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F19" s="14" t="s">
         <v>37</v>
@@ -1779,15 +1779,15 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F20" s="14" t="s">
         <v>37</v>
@@ -1803,10 +1803,10 @@
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F21" s="14" t="s">
         <v>37</v>
@@ -1817,15 +1817,15 @@
     </row>
     <row r="22" spans="1:7" hidden="1">
       <c r="A22" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F22" s="14" t="s">
         <v>37</v>
@@ -1841,10 +1841,10 @@
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>37</v>
@@ -1855,15 +1855,15 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F24" s="17" t="s">
         <v>37</v>
@@ -1884,10 +1884,10 @@
         <v>20</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>30</v>
@@ -1905,35 +1905,35 @@
         <v>14</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F26" s="12" t="s">
         <v>30</v>
       </c>
       <c r="G26" s="2" t="str">
-        <f>"-1 Treasure, +3 Actives"</f>
-        <v>-1 Treasure, +3 Actives</v>
+        <f>"-1 Treasure, +3 Active"</f>
+        <v>-1 Treasure, +3 Active</v>
       </c>
     </row>
     <row r="27" spans="1:7" hidden="1">
       <c r="A27" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F27" s="12" t="s">
         <v>30</v>
@@ -1945,17 +1945,17 @@
     </row>
     <row r="28" spans="1:7" hidden="1">
       <c r="A28" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>30</v>
@@ -1967,17 +1967,17 @@
     </row>
     <row r="29" spans="1:7" hidden="1">
       <c r="A29" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B29" s="16"/>
       <c r="C29" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>30</v>
@@ -1989,17 +1989,17 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8" t="s">
         <v>68</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>30</v>
@@ -2020,10 +2020,10 @@
         <v>21</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>30</v>
@@ -2035,17 +2035,17 @@
     </row>
     <row r="32" spans="1:7" hidden="1">
       <c r="A32" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B32" s="16"/>
       <c r="C32" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>30</v>
@@ -2066,10 +2066,10 @@
         <v>24</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>30</v>
@@ -2081,17 +2081,17 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="8" t="s">
         <v>64</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>30</v>
@@ -2112,10 +2112,10 @@
         <v>20</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>28</v>
@@ -2127,17 +2127,17 @@
     </row>
     <row r="36" spans="1:7" hidden="1">
       <c r="A36" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B36" s="16"/>
       <c r="C36" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F36" s="9" t="s">
         <v>28</v>
@@ -2149,17 +2149,17 @@
     </row>
     <row r="37" spans="1:7" hidden="1">
       <c r="A37" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B37" s="16"/>
       <c r="C37" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F37" s="9" t="s">
         <v>28</v>
@@ -2171,19 +2171,19 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F38" s="9" t="s">
         <v>28</v>
@@ -2204,10 +2204,10 @@
         <v>21</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F39" s="9" t="s">
         <v>28</v>
@@ -2226,10 +2226,10 @@
         <v>21</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F40" s="9" t="s">
         <v>28</v>
@@ -2248,10 +2248,10 @@
         <v>21</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F41" s="9" t="s">
         <v>28</v>
@@ -2263,17 +2263,17 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F42" s="9" t="s">
         <v>28</v>
@@ -2285,17 +2285,17 @@
     </row>
     <row r="43" spans="1:7" hidden="1">
       <c r="A43" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="8" t="s">
         <v>54</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F43" s="9" t="s">
         <v>28</v>
@@ -2316,10 +2316,10 @@
         <v>20</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F44" s="10" t="s">
         <v>47</v>
@@ -2331,17 +2331,17 @@
     </row>
     <row r="45" spans="1:7" hidden="1">
       <c r="A45" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B45" s="16"/>
       <c r="C45" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F45" s="18" t="s">
         <v>47</v>
@@ -2353,17 +2353,17 @@
     </row>
     <row r="46" spans="1:7" hidden="1">
       <c r="A46" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B46" s="16"/>
       <c r="C46" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F46" s="18" t="s">
         <v>47</v>
@@ -2384,10 +2384,10 @@
         <v>21</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F47" s="10" t="s">
         <v>47</v>
@@ -2399,7 +2399,7 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>26</v>
@@ -2408,10 +2408,10 @@
         <v>21</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>47</v>
@@ -2430,10 +2430,10 @@
         <v>21</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E49" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F49" s="10" t="s">
         <v>47</v>
@@ -2452,10 +2452,10 @@
         <v>21</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F50" s="10" t="s">
         <v>47</v>
@@ -2467,17 +2467,17 @@
     </row>
     <row r="51" spans="1:7" hidden="1">
       <c r="A51" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B51" s="16"/>
       <c r="C51" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F51" s="18" t="s">
         <v>47</v>
@@ -2496,10 +2496,10 @@
         <v>57</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>47</v>
@@ -2518,17 +2518,17 @@
         <v>20</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E53" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F53" s="11" t="s">
         <v>29</v>
       </c>
       <c r="G53" s="8" t="str">
-        <f>"Destroy 1 Jungle to build this, -1 Food, +3 Actives"</f>
-        <v>Destroy 1 Jungle to build this, -1 Food, +3 Actives</v>
+        <f>"Destroy 1 Jungle to build this, -1 Food, +3 Active"</f>
+        <v>Destroy 1 Jungle to build this, -1 Food, +3 Active</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -2542,17 +2542,17 @@
         <v>20</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F54" s="11" t="s">
         <v>29</v>
       </c>
       <c r="G54" s="2" t="str">
-        <f>"-1 Food, +2 Actives"</f>
-        <v>-1 Food, +2 Actives</v>
+        <f>"-1 Food, +2 Active"</f>
+        <v>-1 Food, +2 Active</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -2561,13 +2561,13 @@
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="8" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F55" s="11" t="s">
         <v>29</v>
@@ -2579,17 +2579,17 @@
     </row>
     <row r="56" spans="1:7" hidden="1">
       <c r="A56" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B56" s="16"/>
       <c r="C56" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F56" s="11" t="s">
         <v>29</v>
@@ -2601,17 +2601,17 @@
     </row>
     <row r="57" spans="1:7" hidden="1">
       <c r="A57" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B57" s="16"/>
       <c r="C57" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E57" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F57" s="11" t="s">
         <v>29</v>
@@ -2632,10 +2632,10 @@
         <v>21</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F58" s="11" t="s">
         <v>29</v>
@@ -2647,7 +2647,7 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="2" t="s">
-        <v>69</v>
+        <v>149</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>17</v>
@@ -2656,17 +2656,17 @@
         <v>22</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F59" s="11" t="s">
         <v>29</v>
       </c>
       <c r="G59" s="2" t="str">
-        <f>"-1 Food, +2 Actives, +1 Material"</f>
-        <v>-1 Food, +2 Actives, +1 Material</v>
+        <f>"-1 Food, +2 Active, +1 Material"</f>
+        <v>-1 Food, +2 Active, +1 Material</v>
       </c>
     </row>
     <row r="60" spans="1:7" hidden="1">
@@ -2680,10 +2680,10 @@
         <v>24</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F60" s="11" t="s">
         <v>29</v>
@@ -2704,30 +2704,30 @@
         <v>24</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F61" s="11" t="s">
         <v>29</v>
       </c>
       <c r="G61" s="8" t="str">
-        <f>"-2 Food, +3 Actives"</f>
-        <v>-2 Food, +3 Actives</v>
+        <f>"-2 Food, +3 Active"</f>
+        <v>-2 Food, +3 Active</v>
       </c>
     </row>
     <row r="62" spans="1:7" hidden="1">
       <c r="A62" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B62" s="16"/>
       <c r="C62" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D62" s="16"/>
       <c r="E62" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F62" s="15" t="s">
         <v>61</v>
@@ -2747,7 +2747,7 @@
       </c>
       <c r="D63" s="8"/>
       <c r="E63" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F63" s="15" t="s">
         <v>61</v>
@@ -2767,7 +2767,7 @@
       </c>
       <c r="D64" s="8"/>
       <c r="E64" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F64" s="15" t="s">
         <v>61</v>
@@ -2787,7 +2787,7 @@
       </c>
       <c r="D65" s="8"/>
       <c r="E65" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F65" s="15" t="s">
         <v>61</v>
@@ -2807,7 +2807,7 @@
       </c>
       <c r="D66" s="8"/>
       <c r="E66" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F66" s="15" t="s">
         <v>61</v>
@@ -2819,7 +2819,7 @@
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B67" s="8"/>
       <c r="C67" s="8" t="s">
@@ -2827,7 +2827,7 @@
       </c>
       <c r="D67" s="8"/>
       <c r="E67" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F67" s="15" t="s">
         <v>61</v>
@@ -2839,7 +2839,7 @@
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B68" s="8"/>
       <c r="C68" s="8" t="s">
@@ -2847,7 +2847,7 @@
       </c>
       <c r="D68" s="8"/>
       <c r="E68" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F68" s="15" t="s">
         <v>61</v>
@@ -2859,7 +2859,7 @@
     </row>
     <row r="69" spans="1:7">
       <c r="A69" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B69" s="8"/>
       <c r="C69" s="8" t="s">
@@ -2867,7 +2867,7 @@
       </c>
       <c r="D69" s="8"/>
       <c r="E69" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F69" s="15" t="s">
         <v>61</v>
@@ -4486,14 +4486,14 @@
       </c>
       <c r="O33" s="34"/>
       <c r="R33" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="10:18" ht="30" customHeight="1">
       <c r="J34" s="32"/>
       <c r="O34" s="26"/>
       <c r="R34" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="10:18" ht="30" customHeight="1">
@@ -4512,7 +4512,7 @@
       </c>
       <c r="O35" s="28"/>
       <c r="R35" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="10:18" ht="30" customHeight="1">
@@ -4535,7 +4535,7 @@
         <v>8</v>
       </c>
       <c r="R36" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="10:18" ht="30" customHeight="1">
@@ -4576,7 +4576,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1">
         <v>3</v>
@@ -4584,7 +4584,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2">
         <v>1.5</v>
@@ -4592,15 +4592,15 @@
     </row>
     <row r="4" spans="1:3">
       <c r="B4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" t="s">
         <v>121</v>
-      </c>
-      <c r="C4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B5">
         <f>0.5*width</f>
@@ -4612,7 +4612,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B6">
         <f>(0.5*width-0.5*height)</f>
@@ -4625,7 +4625,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B7">
         <f>-(0.5*width-0.5*height)</f>
@@ -4638,7 +4638,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B8">
         <v>-1.5</v>
@@ -4649,7 +4649,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B9">
         <f>-(0.5*width-0.5*height)</f>
@@ -4662,7 +4662,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B10">
         <f>(0.5*width-0.5*height)</f>
@@ -4696,7 +4696,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.75">
       <c r="A1" s="50" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B1" s="50"/>
     </row>
@@ -4705,7 +4705,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4713,7 +4713,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="49" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30">
@@ -4721,7 +4721,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30">
@@ -4729,7 +4729,7 @@
         <v>3.1</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30">
@@ -4737,7 +4737,7 @@
         <v>3.2</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30">
@@ -4745,7 +4745,7 @@
         <v>3.3</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30">
@@ -4753,7 +4753,7 @@
         <v>3.4</v>
       </c>
       <c r="B8" s="47" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="45">
@@ -4761,7 +4761,7 @@
         <v>3.5</v>
       </c>
       <c r="B9" s="47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="45">
@@ -4769,7 +4769,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30">
@@ -4777,7 +4777,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Beginnings of development description popup
</commit_message>
<xml_diff>
--- a/SettleGame.xlsx
+++ b/SettleGame.xlsx
@@ -173,12 +173,6 @@
     <t>Pilgrim Ship</t>
   </si>
   <si>
-    <t>4T</t>
-  </si>
-  <si>
-    <t>7F</t>
-  </si>
-  <si>
     <t>7M</t>
   </si>
   <si>
@@ -188,12 +182,6 @@
     <t>3M</t>
   </si>
   <si>
-    <t>2T</t>
-  </si>
-  <si>
-    <t>4F</t>
-  </si>
-  <si>
     <t>4M</t>
   </si>
   <si>
@@ -471,6 +459,18 @@
   </si>
   <si>
     <t>Shepherd Village</t>
+  </si>
+  <si>
+    <t>6F, 2M</t>
+  </si>
+  <si>
+    <t>3T, 2M</t>
+  </si>
+  <si>
+    <t>2T, 1M</t>
+  </si>
+  <si>
+    <t>4F, 1M</t>
   </si>
 </sst>
 </file>
@@ -1514,8 +1514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1533,7 +1533,7 @@
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
@@ -1555,7 +1555,7 @@
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -1568,7 +1568,7 @@
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
@@ -1607,7 +1607,7 @@
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -1625,11 +1625,11 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="6" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1638,10 +1638,10 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -1650,11 +1650,11 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
@@ -1663,11 +1663,11 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -1676,11 +1676,11 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
@@ -1689,11 +1689,11 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -1702,11 +1702,11 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1746,10 +1746,10 @@
         <v>9</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>27</v>
@@ -1760,15 +1760,15 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F19" s="14" t="s">
         <v>37</v>
@@ -1779,15 +1779,15 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F20" s="14" t="s">
         <v>37</v>
@@ -1803,10 +1803,10 @@
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F21" s="14" t="s">
         <v>37</v>
@@ -1817,15 +1817,15 @@
     </row>
     <row r="22" spans="1:7" hidden="1">
       <c r="A22" s="16" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F22" s="14" t="s">
         <v>37</v>
@@ -1836,15 +1836,15 @@
     </row>
     <row r="23" spans="1:7" hidden="1">
       <c r="A23" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>37</v>
@@ -1855,15 +1855,15 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F24" s="17" t="s">
         <v>37</v>
@@ -1884,10 +1884,10 @@
         <v>20</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>30</v>
@@ -1899,19 +1899,19 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F26" s="12" t="s">
         <v>30</v>
@@ -1923,17 +1923,17 @@
     </row>
     <row r="27" spans="1:7" hidden="1">
       <c r="A27" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F27" s="12" t="s">
         <v>30</v>
@@ -1945,17 +1945,17 @@
     </row>
     <row r="28" spans="1:7" hidden="1">
       <c r="A28" s="16" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="16" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>30</v>
@@ -1967,17 +1967,17 @@
     </row>
     <row r="29" spans="1:7" hidden="1">
       <c r="A29" s="16" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B29" s="16"/>
       <c r="C29" s="16" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>30</v>
@@ -1989,17 +1989,17 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>30</v>
@@ -2011,7 +2011,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>25</v>
@@ -2020,10 +2020,10 @@
         <v>21</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>30</v>
@@ -2035,17 +2035,17 @@
     </row>
     <row r="32" spans="1:7" hidden="1">
       <c r="A32" s="16" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B32" s="16"/>
       <c r="C32" s="16" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>30</v>
@@ -2066,10 +2066,10 @@
         <v>24</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>30</v>
@@ -2081,17 +2081,17 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>30</v>
@@ -2112,10 +2112,10 @@
         <v>20</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>28</v>
@@ -2127,17 +2127,17 @@
     </row>
     <row r="36" spans="1:7" hidden="1">
       <c r="A36" s="16" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B36" s="16"/>
       <c r="C36" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F36" s="9" t="s">
         <v>28</v>
@@ -2149,17 +2149,17 @@
     </row>
     <row r="37" spans="1:7" hidden="1">
       <c r="A37" s="16" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B37" s="16"/>
       <c r="C37" s="16" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F37" s="9" t="s">
         <v>28</v>
@@ -2171,19 +2171,19 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F38" s="9" t="s">
         <v>28</v>
@@ -2204,10 +2204,10 @@
         <v>21</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F39" s="9" t="s">
         <v>28</v>
@@ -2226,10 +2226,10 @@
         <v>21</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F40" s="9" t="s">
         <v>28</v>
@@ -2241,17 +2241,17 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F41" s="9" t="s">
         <v>28</v>
@@ -2263,17 +2263,17 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F42" s="9" t="s">
         <v>28</v>
@@ -2285,17 +2285,17 @@
     </row>
     <row r="43" spans="1:7" hidden="1">
       <c r="A43" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F43" s="9" t="s">
         <v>28</v>
@@ -2316,10 +2316,10 @@
         <v>20</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F44" s="10" t="s">
         <v>47</v>
@@ -2331,17 +2331,17 @@
     </row>
     <row r="45" spans="1:7" hidden="1">
       <c r="A45" s="16" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B45" s="16"/>
       <c r="C45" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F45" s="18" t="s">
         <v>47</v>
@@ -2353,17 +2353,17 @@
     </row>
     <row r="46" spans="1:7" hidden="1">
       <c r="A46" s="16" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B46" s="16"/>
       <c r="C46" s="16" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F46" s="18" t="s">
         <v>47</v>
@@ -2384,10 +2384,10 @@
         <v>21</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F47" s="10" t="s">
         <v>47</v>
@@ -2399,7 +2399,7 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>26</v>
@@ -2408,10 +2408,10 @@
         <v>21</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>47</v>
@@ -2430,10 +2430,10 @@
         <v>21</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E49" s="16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F49" s="10" t="s">
         <v>47</v>
@@ -2452,10 +2452,10 @@
         <v>21</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F50" s="10" t="s">
         <v>47</v>
@@ -2467,17 +2467,17 @@
     </row>
     <row r="51" spans="1:7" hidden="1">
       <c r="A51" s="16" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B51" s="16"/>
       <c r="C51" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F51" s="18" t="s">
         <v>47</v>
@@ -2489,17 +2489,17 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>47</v>
@@ -2518,10 +2518,10 @@
         <v>20</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E53" s="16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F53" s="11" t="s">
         <v>29</v>
@@ -2533,7 +2533,7 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>13</v>
@@ -2542,10 +2542,10 @@
         <v>20</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F54" s="11" t="s">
         <v>29</v>
@@ -2557,17 +2557,17 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F55" s="11" t="s">
         <v>29</v>
@@ -2579,17 +2579,17 @@
     </row>
     <row r="56" spans="1:7" hidden="1">
       <c r="A56" s="16" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B56" s="16"/>
       <c r="C56" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F56" s="11" t="s">
         <v>29</v>
@@ -2601,17 +2601,17 @@
     </row>
     <row r="57" spans="1:7" hidden="1">
       <c r="A57" s="16" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B57" s="16"/>
       <c r="C57" s="16" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E57" s="16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F57" s="11" t="s">
         <v>29</v>
@@ -2632,10 +2632,10 @@
         <v>21</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F58" s="11" t="s">
         <v>29</v>
@@ -2647,7 +2647,7 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>17</v>
@@ -2656,10 +2656,10 @@
         <v>22</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F59" s="11" t="s">
         <v>29</v>
@@ -2680,10 +2680,10 @@
         <v>24</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F60" s="11" t="s">
         <v>29</v>
@@ -2704,10 +2704,10 @@
         <v>24</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F61" s="11" t="s">
         <v>29</v>
@@ -2719,18 +2719,18 @@
     </row>
     <row r="62" spans="1:7" hidden="1">
       <c r="A62" s="16" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B62" s="16"/>
       <c r="C62" s="16" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D62" s="16"/>
       <c r="E62" s="16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F62" s="15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G62" s="16" t="str">
         <f>"Destroy 2 Black developments to build this, +1 Ship"</f>
@@ -2743,14 +2743,14 @@
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="8" t="s">
-        <v>55</v>
+        <v>148</v>
       </c>
       <c r="D63" s="8"/>
       <c r="E63" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F63" s="15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G63" s="8" t="str">
         <f>"Destroy 1 Blue development to build this, +1 Ship"</f>
@@ -2763,14 +2763,14 @@
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="8" t="s">
-        <v>56</v>
+        <v>149</v>
       </c>
       <c r="D64" s="8"/>
       <c r="E64" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F64" s="15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G64" s="8" t="str">
         <f>"Destroy 1 Green development to build this, +1 Ship"</f>
@@ -2783,14 +2783,14 @@
       </c>
       <c r="B65" s="8"/>
       <c r="C65" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D65" s="8"/>
       <c r="E65" s="16" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F65" s="15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G65" s="8" t="str">
         <f>"Destroy 1 Red development to build this, +2 Ships"</f>
@@ -2803,14 +2803,14 @@
       </c>
       <c r="B66" s="8"/>
       <c r="C66" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D66" s="8"/>
       <c r="E66" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F66" s="15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G66" s="8" t="str">
         <f>"Destroy 1 Orange development to build this, +1 Ship"</f>
@@ -2819,18 +2819,18 @@
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B67" s="8"/>
       <c r="C67" s="8" t="s">
-        <v>50</v>
+        <v>147</v>
       </c>
       <c r="D67" s="8"/>
       <c r="E67" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F67" s="15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G67" s="8" t="str">
         <f>"+1 Ship"</f>
@@ -2839,18 +2839,18 @@
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B68" s="8"/>
       <c r="C68" s="8" t="s">
-        <v>51</v>
+        <v>146</v>
       </c>
       <c r="D68" s="8"/>
       <c r="E68" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F68" s="15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G68" s="8" t="str">
         <f>"+1 Ship"</f>
@@ -2859,18 +2859,18 @@
     </row>
     <row r="69" spans="1:7">
       <c r="A69" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B69" s="8"/>
       <c r="C69" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D69" s="8"/>
       <c r="E69" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F69" s="15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G69" s="8" t="str">
         <f>"+1 Ship"</f>
@@ -4486,14 +4486,14 @@
       </c>
       <c r="O33" s="34"/>
       <c r="R33" s="19" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="10:18" ht="30" customHeight="1">
       <c r="J34" s="32"/>
       <c r="O34" s="26"/>
       <c r="R34" s="19" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="10:18" ht="30" customHeight="1">
@@ -4512,7 +4512,7 @@
       </c>
       <c r="O35" s="28"/>
       <c r="R35" s="19" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="10:18" ht="30" customHeight="1">
@@ -4535,7 +4535,7 @@
         <v>8</v>
       </c>
       <c r="R36" s="19" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="10:18" ht="30" customHeight="1">
@@ -4576,7 +4576,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B1">
         <v>3</v>
@@ -4584,7 +4584,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B2">
         <v>1.5</v>
@@ -4592,15 +4592,15 @@
     </row>
     <row r="4" spans="1:3">
       <c r="B4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B5">
         <f>0.5*width</f>
@@ -4612,7 +4612,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B6">
         <f>(0.5*width-0.5*height)</f>
@@ -4625,7 +4625,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B7">
         <f>-(0.5*width-0.5*height)</f>
@@ -4638,7 +4638,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B8">
         <v>-1.5</v>
@@ -4649,7 +4649,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B9">
         <f>-(0.5*width-0.5*height)</f>
@@ -4662,7 +4662,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B10">
         <f>(0.5*width-0.5*height)</f>
@@ -4696,7 +4696,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.75">
       <c r="A1" s="50" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B1" s="50"/>
     </row>
@@ -4705,7 +4705,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4713,7 +4713,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="49" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30">
@@ -4721,7 +4721,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30">
@@ -4729,7 +4729,7 @@
         <v>3.1</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30">
@@ -4737,7 +4737,7 @@
         <v>3.2</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30">
@@ -4745,7 +4745,7 @@
         <v>3.3</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30">
@@ -4753,7 +4753,7 @@
         <v>3.4</v>
       </c>
       <c r="B8" s="47" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="45">
@@ -4761,7 +4761,7 @@
         <v>3.5</v>
       </c>
       <c r="B9" s="47" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="45">
@@ -4769,7 +4769,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30">
@@ -4777,7 +4777,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Additions to concept spreadsheet
</commit_message>
<xml_diff>
--- a/SettleGame.xlsx
+++ b/SettleGame.xlsx
@@ -1,27 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmatthews\Documents\JS\Archipelago\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="17925" windowHeight="6645"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="17925" windowHeight="6645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="1" r:id="rId1"/>
     <sheet name="Mapping" sheetId="2" r:id="rId2"/>
     <sheet name="Hexagons" sheetId="3" r:id="rId3"/>
     <sheet name="RandGen" sheetId="4" r:id="rId4"/>
+    <sheet name="Ideas" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="height">Hexagons!$B$2</definedName>
     <definedName name="width">Hexagons!$B$1</definedName>
   </definedNames>
-  <calcPr calcId="125725" calcOnSave="0"/>
+  <calcPr calcId="162913" calcMode="manual" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="186">
   <si>
     <t>Conceit</t>
   </si>
@@ -212,9 +218,6 @@
     <t>Cobalt Mine</t>
   </si>
   <si>
-    <t>Rocky Shore</t>
-  </si>
-  <si>
     <t>2F, 2M, 2T</t>
   </si>
   <si>
@@ -471,13 +474,124 @@
   </si>
   <si>
     <t>4F, 1M</t>
+  </si>
+  <si>
+    <t>Thematic</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Cliffs</t>
+  </si>
+  <si>
+    <t>Lighthouse</t>
+  </si>
+  <si>
+    <t>Larder</t>
+  </si>
+  <si>
+    <t>No Food spoilage next month</t>
+  </si>
+  <si>
+    <t>No Material spoilage next month</t>
+  </si>
+  <si>
+    <t>Build one development without using an action</t>
+  </si>
+  <si>
+    <t>Increase buid distance for this month</t>
+  </si>
+  <si>
+    <t>Storehouse</t>
+  </si>
+  <si>
+    <t>Aviary</t>
+  </si>
+  <si>
+    <t>Metalsmith</t>
+  </si>
+  <si>
+    <t>Sluice</t>
+  </si>
+  <si>
+    <t>Windmill</t>
+  </si>
+  <si>
+    <t>Watermill</t>
+  </si>
+  <si>
+    <t>Palace</t>
+  </si>
+  <si>
+    <t>Watchtower</t>
+  </si>
+  <si>
+    <t>View/re-order upcoming developments</t>
+  </si>
+  <si>
+    <t>Mushroom Farm</t>
+  </si>
+  <si>
+    <t>Coconut Grove</t>
+  </si>
+  <si>
+    <t>Mechanics</t>
+  </si>
+  <si>
+    <t>Developments that generate things every month, without needing to be used</t>
+  </si>
+  <si>
+    <t>Graveyard</t>
+  </si>
+  <si>
+    <t>Bath House</t>
+  </si>
+  <si>
+    <t>Rebuild destroyed development</t>
+  </si>
+  <si>
+    <t>Observatory</t>
+  </si>
+  <si>
+    <t>Cloth Market</t>
+  </si>
+  <si>
+    <t>Events, which are smaller goals that both players attempts to achieve:</t>
+  </si>
+  <si>
+    <t>Build on a certain space equidistant from either player</t>
+  </si>
+  <si>
+    <t>Destroys itself when used</t>
+  </si>
+  <si>
+    <t>Circus</t>
+  </si>
+  <si>
+    <t>Destroy the most developments</t>
+  </si>
+  <si>
+    <t>Tournament</t>
+  </si>
+  <si>
+    <t>Decrease development cost</t>
+  </si>
+  <si>
+    <t>Gain the most territory</t>
+  </si>
+  <si>
+    <t>Build most valuable development</t>
+  </si>
+  <si>
+    <t>Control the most black developments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -808,7 +922,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -889,6 +1003,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1036,18 +1151,40 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
-    <c:title/>
+    <c:title>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1121,7 +1258,21 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BF1C-4F0E-B068-D899AF203BFB}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:axId val="80375168"/>
         <c:axId val="80630912"/>
       </c:scatterChart>
@@ -1130,8 +1281,11 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="80630912"/>
         <c:crosses val="autoZero"/>
@@ -1142,9 +1296,12 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="80375168"/>
         <c:crosses val="autoZero"/>
@@ -1153,8 +1310,11 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1201,16 +1361,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A18:G69" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A18:G69">
-    <filterColumn colId="1"/>
-    <filterColumn colId="3"/>
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Basic"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="5"/>
-  </autoFilter>
+  <autoFilter ref="A18:G69"/>
   <sortState ref="A19:G69">
     <sortCondition ref="F18:F69"/>
   </sortState>
@@ -1270,7 +1421,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1302,9 +1453,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1336,6 +1488,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1511,14 +1664,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="14" hidden="1" customWidth="1"/>
@@ -1527,20 +1680,20 @@
     <col min="7" max="7" width="99.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
@@ -1549,33 +1702,33 @@
       <c r="F2" s="2"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
@@ -1588,7 +1741,7 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
@@ -1601,7 +1754,7 @@
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>44</v>
       </c>
@@ -1614,7 +1767,7 @@
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -1623,97 +1776,97 @@
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1722,20 +1875,20 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
@@ -1746,10 +1899,10 @@
         <v>9</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>27</v>
@@ -1758,17 +1911,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F19" s="14" t="s">
         <v>37</v>
@@ -1777,17 +1930,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F20" s="14" t="s">
         <v>37</v>
@@ -1796,17 +1949,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F21" s="14" t="s">
         <v>37</v>
@@ -1815,17 +1968,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F22" s="14" t="s">
         <v>37</v>
@@ -1834,17 +1987,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>63</v>
+        <v>151</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>37</v>
@@ -1853,17 +2006,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F24" s="17" t="s">
         <v>37</v>
@@ -1873,7 +2026,7 @@
         <v>+1 Food, +1 Material</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>31</v>
       </c>
@@ -1884,10 +2037,10 @@
         <v>20</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>30</v>
@@ -1897,7 +2050,7 @@
         <v>Destroy Development, +1 Active</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>56</v>
       </c>
@@ -1905,13 +2058,13 @@
         <v>14</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F26" s="12" t="s">
         <v>30</v>
@@ -1921,19 +2074,19 @@
         <v>-1 Treasure, +3 Active</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F27" s="12" t="s">
         <v>30</v>
@@ -1943,19 +2096,19 @@
         <v>-2 Treasure, build any development</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>30</v>
@@ -1965,41 +2118,41 @@
         <v>Destroy a Black development, +2 Material</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B29" s="16"/>
       <c r="C29" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>30</v>
       </c>
       <c r="G29" s="16" t="str">
-        <f xml:space="preserve"> "Destroy a Black development, +2 Food"</f>
-        <v>Destroy a Black development, +2 Food</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <f xml:space="preserve"> "Destroy a Black development, +3 Food"</f>
+        <v>Destroy a Black development, +3 Food</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>30</v>
@@ -2009,7 +2162,7 @@
         <v>-1 Material, For the rest of the month, all Blue developments give an additional +1 Treasure</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>55</v>
       </c>
@@ -2020,10 +2173,10 @@
         <v>21</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>30</v>
@@ -2033,19 +2186,19 @@
         <v>-1 Food, -1 Material, +1 Treasure</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B32" s="16"/>
       <c r="C32" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>30</v>
@@ -2055,7 +2208,7 @@
         <v>Build a Base Camp on any Shore, destroy this Journey Pier</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>23</v>
       </c>
@@ -2066,10 +2219,10 @@
         <v>24</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>30</v>
@@ -2079,19 +2232,19 @@
         <v>-1 Treasure, +2 Treasure</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="8" t="s">
         <v>60</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>30</v>
@@ -2101,7 +2254,7 @@
         <v>-1 Treasure, +2 Food, +2 Material</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
@@ -2112,10 +2265,10 @@
         <v>20</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>28</v>
@@ -2125,19 +2278,19 @@
         <v>+1 Food</v>
       </c>
     </row>
-    <row r="36" spans="1:7" hidden="1">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B36" s="16"/>
       <c r="C36" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F36" s="9" t="s">
         <v>28</v>
@@ -2147,19 +2300,19 @@
         <v>For the rest of the month, Jungle, Cave, and Bog give +1 Food when used</v>
       </c>
     </row>
-    <row r="37" spans="1:7" hidden="1">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B37" s="16"/>
       <c r="C37" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F37" s="9" t="s">
         <v>28</v>
@@ -2169,21 +2322,21 @@
         <v>Build a Jungle on Forested land, +1 Active</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F38" s="9" t="s">
         <v>28</v>
@@ -2193,7 +2346,7 @@
         <v>-1 Food, +3 Food</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>36</v>
       </c>
@@ -2204,10 +2357,10 @@
         <v>21</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F39" s="9" t="s">
         <v>28</v>
@@ -2217,7 +2370,7 @@
         <v>+1 Food, +1 Active</v>
       </c>
     </row>
-    <row r="40" spans="1:7" hidden="1">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>48</v>
       </c>
@@ -2226,10 +2379,10 @@
         <v>21</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F40" s="9" t="s">
         <v>28</v>
@@ -2239,7 +2392,7 @@
         <v>Destroy 1 Freshwater to build this, +1 Food, +1 Material</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>59</v>
       </c>
@@ -2248,10 +2401,10 @@
         <v>21</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F41" s="9" t="s">
         <v>28</v>
@@ -2261,19 +2414,19 @@
         <v>-1 Material, +3 Food</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F42" s="9" t="s">
         <v>28</v>
@@ -2283,19 +2436,19 @@
         <v>+2 Food</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="8" t="s">
         <v>52</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F43" s="9" t="s">
         <v>28</v>
@@ -2305,7 +2458,7 @@
         <v>-1 Active, +1 Treasure</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>34</v>
       </c>
@@ -2316,10 +2469,10 @@
         <v>20</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F44" s="10" t="s">
         <v>47</v>
@@ -2329,19 +2482,19 @@
         <v>+1 Material</v>
       </c>
     </row>
-    <row r="45" spans="1:7" hidden="1">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B45" s="16"/>
       <c r="C45" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F45" s="18" t="s">
         <v>47</v>
@@ -2351,19 +2504,19 @@
         <v>Build another Rope Weaver</v>
       </c>
     </row>
-    <row r="46" spans="1:7" hidden="1">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B46" s="16"/>
       <c r="C46" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E46" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F46" s="18" t="s">
         <v>47</v>
@@ -2373,7 +2526,7 @@
         <v>Build a Cave on Rocky land, +1 Active</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>41</v>
       </c>
@@ -2384,10 +2537,10 @@
         <v>21</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F47" s="10" t="s">
         <v>47</v>
@@ -2397,9 +2550,9 @@
         <v>-2 Food, +1 Treasure</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>26</v>
@@ -2408,10 +2561,10 @@
         <v>21</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>47</v>
@@ -2421,7 +2574,7 @@
         <v>-1 Food, +3 Material</v>
       </c>
     </row>
-    <row r="49" spans="1:7" hidden="1">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>42</v>
       </c>
@@ -2430,10 +2583,10 @@
         <v>21</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E49" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F49" s="10" t="s">
         <v>47</v>
@@ -2443,7 +2596,7 @@
         <v>Destroy 1 Cave to build this, +1 Treasure</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>12</v>
       </c>
@@ -2452,10 +2605,10 @@
         <v>21</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F50" s="10" t="s">
         <v>47</v>
@@ -2465,19 +2618,19 @@
         <v>+2 Material</v>
       </c>
     </row>
-    <row r="51" spans="1:7" hidden="1">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B51" s="16"/>
       <c r="C51" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F51" s="18" t="s">
         <v>47</v>
@@ -2487,7 +2640,7 @@
         <v>+1 Material</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>62</v>
       </c>
@@ -2496,10 +2649,10 @@
         <v>53</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>47</v>
@@ -2509,7 +2662,7 @@
         <v>+1 Treasure</v>
       </c>
     </row>
-    <row r="53" spans="1:7" hidden="1">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>40</v>
       </c>
@@ -2518,10 +2671,10 @@
         <v>20</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E53" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F53" s="11" t="s">
         <v>29</v>
@@ -2531,7 +2684,7 @@
         <v>Destroy 1 Jungle to build this, -1 Food, +3 Active</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>58</v>
       </c>
@@ -2542,10 +2695,10 @@
         <v>20</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F54" s="11" t="s">
         <v>29</v>
@@ -2555,19 +2708,19 @@
         <v>-1 Food, +2 Active</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>61</v>
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F55" s="11" t="s">
         <v>29</v>
@@ -2577,19 +2730,19 @@
         <v>-1 Food, For the rest of the month, all Red developments give an additional +1 Active</v>
       </c>
     </row>
-    <row r="56" spans="1:7" hidden="1">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B56" s="16"/>
       <c r="C56" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E56" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F56" s="11" t="s">
         <v>29</v>
@@ -2599,19 +2752,19 @@
         <v>+1 Active</v>
       </c>
     </row>
-    <row r="57" spans="1:7" hidden="1">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B57" s="16"/>
       <c r="C57" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E57" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F57" s="11" t="s">
         <v>29</v>
@@ -2621,7 +2774,7 @@
         <v>+1 Active, Perform the effect of an adjacent development</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -2632,10 +2785,10 @@
         <v>21</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F58" s="11" t="s">
         <v>29</v>
@@ -2645,9 +2798,9 @@
         <v>Destroy development, +1 Material</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>17</v>
@@ -2656,10 +2809,10 @@
         <v>22</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F59" s="11" t="s">
         <v>29</v>
@@ -2669,7 +2822,7 @@
         <v>-1 Food, +2 Active, +1 Material</v>
       </c>
     </row>
-    <row r="60" spans="1:7" hidden="1">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>19</v>
       </c>
@@ -2680,10 +2833,10 @@
         <v>24</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E60" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F60" s="11" t="s">
         <v>29</v>
@@ -2693,7 +2846,7 @@
         <v>-1 Food, Destroy a non-Black development, Replace with any non-Violet development</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>35</v>
       </c>
@@ -2704,10 +2857,10 @@
         <v>24</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F61" s="11" t="s">
         <v>29</v>
@@ -2717,17 +2870,17 @@
         <v>-2 Food, +3 Active</v>
       </c>
     </row>
-    <row r="62" spans="1:7" hidden="1">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B62" s="16"/>
       <c r="C62" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D62" s="16"/>
       <c r="E62" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F62" s="15" t="s">
         <v>57</v>
@@ -2737,17 +2890,17 @@
         <v>Destroy 2 Black developments to build this, +1 Ship</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D63" s="8"/>
       <c r="E63" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F63" s="15" t="s">
         <v>57</v>
@@ -2757,17 +2910,17 @@
         <v>Destroy 1 Blue development to build this, +1 Ship</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>45</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D64" s="8"/>
       <c r="E64" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F64" s="15" t="s">
         <v>57</v>
@@ -2777,7 +2930,7 @@
         <v>Destroy 1 Green development to build this, +1 Ship</v>
       </c>
     </row>
-    <row r="65" spans="1:7" hidden="1">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>49</v>
       </c>
@@ -2787,7 +2940,7 @@
       </c>
       <c r="D65" s="8"/>
       <c r="E65" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F65" s="15" t="s">
         <v>57</v>
@@ -2797,7 +2950,7 @@
         <v>Destroy 1 Red development to build this, +2 Ships</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
         <v>46</v>
       </c>
@@ -2807,7 +2960,7 @@
       </c>
       <c r="D66" s="8"/>
       <c r="E66" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F66" s="15" t="s">
         <v>57</v>
@@ -2817,17 +2970,17 @@
         <v>Destroy 1 Orange development to build this, +1 Ship</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B67" s="8"/>
       <c r="C67" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D67" s="8"/>
       <c r="E67" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F67" s="15" t="s">
         <v>57</v>
@@ -2837,17 +2990,17 @@
         <v>+1 Ship</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B68" s="8"/>
       <c r="C68" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D68" s="8"/>
       <c r="E68" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F68" s="15" t="s">
         <v>57</v>
@@ -2857,9 +3010,9 @@
         <v>+1 Ship</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B69" s="8"/>
       <c r="C69" s="8" t="s">
@@ -2867,7 +3020,7 @@
       </c>
       <c r="D69" s="8"/>
       <c r="E69" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F69" s="15" t="s">
         <v>57</v>
@@ -2887,20 +3040,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE38"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" style="19" customWidth="1"/>
     <col min="2" max="16384" width="5.7109375" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="30" customHeight="1">
+    <row r="1" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22">
         <v>0</v>
       </c>
@@ -2962,7 +3115,7 @@
       </c>
       <c r="AD1" s="21"/>
     </row>
-    <row r="2" spans="1:31" ht="30" customHeight="1">
+    <row r="2" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22">
         <v>-9</v>
       </c>
@@ -3057,7 +3210,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="30" customHeight="1">
+    <row r="3" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22">
         <v>-8</v>
       </c>
@@ -3147,7 +3300,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="30" customHeight="1">
+    <row r="4" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24">
         <v>-7</v>
       </c>
@@ -3242,7 +3395,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="30" customHeight="1">
+    <row r="5" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22">
         <v>-6</v>
       </c>
@@ -3332,7 +3485,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="30" customHeight="1">
+    <row r="6" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22">
         <v>-5</v>
       </c>
@@ -3427,7 +3580,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:31" ht="30" customHeight="1">
+    <row r="7" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24">
         <v>-4</v>
       </c>
@@ -3517,7 +3670,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="30" customHeight="1">
+    <row r="8" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22">
         <v>-3</v>
       </c>
@@ -3612,7 +3765,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="30" customHeight="1">
+    <row r="9" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22">
         <v>-2</v>
       </c>
@@ -3702,7 +3855,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="30" customHeight="1">
+    <row r="10" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24">
         <v>-1</v>
       </c>
@@ -3797,7 +3950,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="30" customHeight="1">
+    <row r="11" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22">
         <v>0</v>
       </c>
@@ -3887,7 +4040,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="30" customHeight="1">
+    <row r="12" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="24">
         <v>1</v>
       </c>
@@ -3982,7 +4135,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="30" customHeight="1">
+    <row r="13" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22">
         <v>2</v>
       </c>
@@ -4072,7 +4225,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="30" customHeight="1">
+    <row r="14" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22">
         <v>3</v>
       </c>
@@ -4167,7 +4320,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="30" customHeight="1">
+    <row r="15" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="24">
         <v>4</v>
       </c>
@@ -4257,7 +4410,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="30" customHeight="1">
+    <row r="16" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22">
         <v>5</v>
       </c>
@@ -4292,7 +4445,7 @@
       <c r="AD16" s="20"/>
       <c r="AE16" s="21"/>
     </row>
-    <row r="17" spans="1:31" ht="30" customHeight="1">
+    <row r="17" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22">
         <v>6</v>
       </c>
@@ -4326,7 +4479,7 @@
       <c r="AC17" s="20"/>
       <c r="AD17" s="21"/>
     </row>
-    <row r="18" spans="1:31" ht="30" customHeight="1">
+    <row r="18" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24">
         <v>7</v>
       </c>
@@ -4361,7 +4514,7 @@
       <c r="AD18" s="20"/>
       <c r="AE18" s="21"/>
     </row>
-    <row r="19" spans="1:31" ht="30" customHeight="1">
+    <row r="19" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22">
         <v>8</v>
       </c>
@@ -4395,7 +4548,7 @@
       <c r="AC19" s="20"/>
       <c r="AD19" s="21"/>
     </row>
-    <row r="20" spans="1:31" ht="30" customHeight="1">
+    <row r="20" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22">
         <v>9</v>
       </c>
@@ -4430,11 +4583,11 @@
       <c r="AD20" s="20"/>
       <c r="AE20" s="21"/>
     </row>
-    <row r="30" spans="1:31" ht="30" customHeight="1">
+    <row r="30" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J30" s="25"/>
       <c r="O30" s="25"/>
     </row>
-    <row r="31" spans="1:31" ht="30" customHeight="1">
+    <row r="31" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J31" s="30"/>
       <c r="K31" s="20">
         <v>-9</v>
@@ -4450,7 +4603,7 @@
       </c>
       <c r="O31" s="31"/>
     </row>
-    <row r="32" spans="1:31" ht="30" customHeight="1">
+    <row r="32" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J32" s="20">
         <v>-8</v>
       </c>
@@ -4470,7 +4623,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="10:18" ht="30" customHeight="1">
+    <row r="33" spans="10:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J33" s="33"/>
       <c r="K33" s="20">
         <v>-7</v>
@@ -4486,17 +4639,17 @@
       </c>
       <c r="O33" s="34"/>
       <c r="R33" s="19" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="34" spans="10:18" ht="30" customHeight="1">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="10:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J34" s="32"/>
       <c r="O34" s="26"/>
       <c r="R34" s="19" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="35" spans="10:18" ht="30" customHeight="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="10:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J35" s="29"/>
       <c r="K35" s="20">
         <v>-8</v>
@@ -4512,10 +4665,10 @@
       </c>
       <c r="O35" s="28"/>
       <c r="R35" s="19" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="36" spans="10:18" ht="30" customHeight="1">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="10:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J36" s="20">
         <v>-7</v>
       </c>
@@ -4535,10 +4688,10 @@
         <v>8</v>
       </c>
       <c r="R36" s="19" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="37" spans="10:18" ht="30" customHeight="1">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="10:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J37" s="35"/>
       <c r="K37" s="20">
         <v>-6</v>
@@ -4554,7 +4707,7 @@
       </c>
       <c r="O37" s="34"/>
     </row>
-    <row r="38" spans="10:18" ht="30" customHeight="1">
+    <row r="38" spans="10:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J38" s="26"/>
       <c r="O38" s="26"/>
     </row>
@@ -4565,42 +4718,42 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B1">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2">
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" t="s">
         <v>116</v>
       </c>
-      <c r="C4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B5">
         <f>0.5*width</f>
@@ -4610,9 +4763,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6">
         <f>(0.5*width-0.5*height)</f>
@@ -4623,9 +4776,9 @@
         <v>-0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B7">
         <f>-(0.5*width-0.5*height)</f>
@@ -4636,9 +4789,9 @@
         <v>-0.75</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B8">
         <v>-1.5</v>
@@ -4647,9 +4800,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B9">
         <f>-(0.5*width-0.5*height)</f>
@@ -4660,9 +4813,9 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B10">
         <f>(0.5*width-0.5*height)</f>
@@ -4680,104 +4833,104 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" style="44" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44" style="45" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75">
-      <c r="A1" s="50" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="50"/>
-    </row>
-    <row r="2" spans="1:2">
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="51" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="51"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="48">
         <v>1</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="48">
         <v>2</v>
       </c>
       <c r="B3" s="49" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="48">
         <v>3</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="30">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="46">
         <v>3.1</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="30">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="46">
         <v>3.2</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="30">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="46">
         <v>3.3</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="30">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="46">
         <v>3.4</v>
       </c>
       <c r="B8" s="47" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="45">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="46">
         <v>3.5</v>
       </c>
       <c r="B9" s="47" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="45">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="48">
         <v>4</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="30">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="48">
         <v>5</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -4787,4 +4940,178 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="44" customWidth="1"/>
+    <col min="4" max="4" width="2.85546875" customWidth="1"/>
+    <col min="5" max="5" width="70.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="50" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" s="50" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C6" t="str">
+        <f>"-# Actions, +# Actions"</f>
+        <v>-# Actions, +# Actions</v>
+      </c>
+      <c r="E6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Continuing active development functionality
</commit_message>
<xml_diff>
--- a/SettleGame.xlsx
+++ b/SettleGame.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="187">
   <si>
     <t>Conceit</t>
   </si>
@@ -497,9 +497,6 @@
     <t>No Material spoilage next month</t>
   </si>
   <si>
-    <t>Build one development without using an action</t>
-  </si>
-  <si>
     <t>Increase buid distance for this month</t>
   </si>
   <si>
@@ -585,6 +582,12 @@
   </si>
   <si>
     <t>Control the most black developments</t>
+  </si>
+  <si>
+    <t>Build black developments regardless of distance</t>
+  </si>
+  <si>
+    <t>Build a development without using an action</t>
   </si>
 </sst>
 </file>
@@ -1667,7 +1670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
@@ -4947,7 +4950,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4968,7 +4971,7 @@
         <v>150</v>
       </c>
       <c r="E1" s="50" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -4979,7 +4982,7 @@
         <v>154</v>
       </c>
       <c r="E2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -4990,124 +4993,127 @@
         <v>155</v>
       </c>
       <c r="E3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
-        <v>156</v>
+        <v>186</v>
       </c>
       <c r="E4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C6" t="str">
         <f>"-# Actions, +# Actions"</f>
         <v>-# Actions, +# Actions</v>
       </c>
       <c r="E6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>164</v>
+        <v>163</v>
+      </c>
+      <c r="C11" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upgrade to Typescript2, typings for PIXI and Tink
</commit_message>
<xml_diff>
--- a/SettleGame.xlsx
+++ b/SettleGame.xlsx
@@ -1,33 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmatthews\Documents\JS\Archipelago\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="17925" windowHeight="6645" activeTab="4"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="24320" windowHeight="14040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="1" r:id="rId1"/>
-    <sheet name="Mapping" sheetId="2" r:id="rId2"/>
-    <sheet name="Hexagons" sheetId="3" r:id="rId3"/>
-    <sheet name="RandGen" sheetId="4" r:id="rId4"/>
-    <sheet name="Ideas" sheetId="5" r:id="rId5"/>
+    <sheet name="Basics v2" sheetId="6" r:id="rId2"/>
+    <sheet name="Mapping" sheetId="2" r:id="rId3"/>
+    <sheet name="Hexagons" sheetId="3" r:id="rId4"/>
+    <sheet name="RandGen" sheetId="4" r:id="rId5"/>
+    <sheet name="Ideas" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="height">Hexagons!$B$2</definedName>
     <definedName name="width">Hexagons!$B$1</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcMode="manual" calcOnSave="0"/>
+  <calcPr calcId="0" calcMode="manual" calcCompleted="0" calcOnSave="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="212">
   <si>
     <t>Conceit</t>
   </si>
@@ -554,9 +555,6 @@
     <t>Cloth Market</t>
   </si>
   <si>
-    <t>Events, which are smaller goals that both players attempts to achieve:</t>
-  </si>
-  <si>
     <t>Build on a certain space equidistant from either player</t>
   </si>
   <si>
@@ -588,13 +586,91 @@
   </si>
   <si>
     <t>Build a development without using an action</t>
+  </si>
+  <si>
+    <t>Events, which are smaller goals that both players attempt to achieve:</t>
+  </si>
+  <si>
+    <t>Effect + when surrounded by other developments</t>
+  </si>
+  <si>
+    <t>Effect - when surrounded by other developments</t>
+  </si>
+  <si>
+    <t>Garden</t>
+  </si>
+  <si>
+    <t>Grove</t>
+  </si>
+  <si>
+    <t>Mercantile</t>
+  </si>
+  <si>
+    <t>2F, 2M</t>
+  </si>
+  <si>
+    <t>Hamlet</t>
+  </si>
+  <si>
+    <t>1F, 2M</t>
+  </si>
+  <si>
+    <t>3F, 3M, 2T</t>
+  </si>
+  <si>
+    <t>2F, 2M, 3T</t>
+  </si>
+  <si>
+    <t>2F, 3M</t>
+  </si>
+  <si>
+    <t>1F, 4M</t>
+  </si>
+  <si>
+    <t>3F, 4M</t>
+  </si>
+  <si>
+    <t>2F, 4M</t>
+  </si>
+  <si>
+    <t>1F, 6M</t>
+  </si>
+  <si>
+    <t>3F, 3M</t>
+  </si>
+  <si>
+    <t>3F, 4M, 1T</t>
+  </si>
+  <si>
+    <t>3M, 3T</t>
+  </si>
+  <si>
+    <t>5M, 5T</t>
+  </si>
+  <si>
+    <t>9F, 4M</t>
+  </si>
+  <si>
+    <t>6F, 6M</t>
+  </si>
+  <si>
+    <t>Grassy, Forested</t>
+  </si>
+  <si>
+    <t>The player who builds the most ships wins, a ship can be built on any sea tile, regardless of distance</t>
+  </si>
+  <si>
+    <t>Effects change based on color of surrounding developments</t>
+  </si>
+  <si>
+    <t>1F, 1M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -658,6 +734,22 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -922,8 +1014,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1011,10 +1123,167 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="21">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF1F497D"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="3"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1166,7 +1435,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1241,7 +1510,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-0.75</c:v>
@@ -1250,7 +1519,7 @@
                   <c:v>-0.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.75</c:v>
@@ -1262,7 +1531,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-BF1C-4F0E-B068-D899AF203BFB}"/>
             </c:ext>
@@ -1276,11 +1545,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="80375168"/>
-        <c:axId val="80630912"/>
+        <c:axId val="2145997192"/>
+        <c:axId val="2145994776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80375168"/>
+        <c:axId val="2145997192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1290,12 +1559,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80630912"/>
+        <c:crossAx val="2145994776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80630912"/>
+        <c:axId val="2145994776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1306,7 +1575,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80375168"/>
+        <c:crossAx val="2145997192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1321,7 +1590,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.700000000000001" r="0.700000000000001" t="0.750000000000001" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1363,8 +1632,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A18:G69" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A18:G69"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A18:G69" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A18:G69">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Basic"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState ref="A19:G69">
+    <sortCondition ref="F18:F69"/>
+  </sortState>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Name" dataDxfId="15"/>
+    <tableColumn id="6" name="Alt Name" dataDxfId="14"/>
+    <tableColumn id="2" name="Cost" dataDxfId="13"/>
+    <tableColumn id="5" name="Place" dataDxfId="12"/>
+    <tableColumn id="7" name="Set" dataDxfId="11"/>
+    <tableColumn id="4" name="Color" dataDxfId="10"/>
+    <tableColumn id="3" name="Effect" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A18:G69" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A18:G69">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Basic"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A19:G69">
     <sortCondition ref="F18:F69"/>
   </sortState>
@@ -1424,7 +1724,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1459,7 +1759,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1670,20 +1970,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="2" max="2" width="14" hidden="1" customWidth="1"/>
-    <col min="3" max="4" width="10.140625" customWidth="1"/>
+    <col min="3" max="4" width="10.1640625" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="99.140625" customWidth="1"/>
+    <col min="7" max="7" width="99.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1696,7 +1996,7 @@
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
@@ -1705,7 +2005,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1718,7 +2018,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
@@ -1731,7 +2031,7 @@
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
@@ -1744,7 +2044,7 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
@@ -1757,7 +2057,7 @@
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="8" t="s">
         <v>44</v>
       </c>
@@ -1770,7 +2070,7 @@
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -1779,7 +2079,7 @@
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="5" t="s">
         <v>82</v>
       </c>
@@ -1792,7 +2092,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="8" t="s">
         <v>78</v>
       </c>
@@ -1804,7 +2104,7 @@
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="8" t="s">
         <v>77</v>
       </c>
@@ -1817,7 +2117,7 @@
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="8" t="s">
         <v>79</v>
       </c>
@@ -1830,7 +2130,7 @@
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="8" t="s">
         <v>81</v>
       </c>
@@ -1843,7 +2143,7 @@
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="8" t="s">
         <v>86</v>
       </c>
@@ -1856,7 +2156,7 @@
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="8" t="s">
         <v>89</v>
       </c>
@@ -1869,7 +2169,7 @@
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1878,7 +2178,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
@@ -1891,7 +2191,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
@@ -1914,7 +2214,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="8" t="s">
         <v>72</v>
       </c>
@@ -1933,7 +2233,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" s="8" t="s">
         <v>128</v>
       </c>
@@ -1952,7 +2252,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="8" t="s">
         <v>39</v>
       </c>
@@ -1971,7 +2271,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" hidden="1">
       <c r="A22" s="16" t="s">
         <v>103</v>
       </c>
@@ -1990,7 +2290,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" hidden="1">
       <c r="A23" s="8" t="s">
         <v>151</v>
       </c>
@@ -2009,7 +2309,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" s="16" t="s">
         <v>73</v>
       </c>
@@ -2029,7 +2329,7 @@
         <v>+1 Food, +1 Material</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" s="8" t="s">
         <v>31</v>
       </c>
@@ -2053,7 +2353,7 @@
         <v>Destroy Development, +1 Active</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" s="2" t="s">
         <v>56</v>
       </c>
@@ -2077,7 +2377,7 @@
         <v>-1 Treasure, +3 Active</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" hidden="1">
       <c r="A27" s="8" t="s">
         <v>68</v>
       </c>
@@ -2099,7 +2399,7 @@
         <v>-2 Treasure, build any development</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" hidden="1">
       <c r="A28" s="16" t="s">
         <v>132</v>
       </c>
@@ -2121,7 +2421,7 @@
         <v>Destroy a Black development, +2 Material</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" hidden="1">
       <c r="A29" s="16" t="s">
         <v>131</v>
       </c>
@@ -2143,7 +2443,7 @@
         <v>Destroy a Black development, +3 Food</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" s="8" t="s">
         <v>70</v>
       </c>
@@ -2165,7 +2465,7 @@
         <v>-1 Material, For the rest of the month, all Blue developments give an additional +1 Treasure</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" s="2" t="s">
         <v>55</v>
       </c>
@@ -2189,7 +2489,7 @@
         <v>-1 Food, -1 Material, +1 Treasure</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" hidden="1">
       <c r="A32" s="16" t="s">
         <v>92</v>
       </c>
@@ -2211,7 +2511,7 @@
         <v>Build a Base Camp on any Shore, destroy this Journey Pier</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="8" t="s">
         <v>23</v>
       </c>
@@ -2235,7 +2535,7 @@
         <v>-1 Treasure, +2 Treasure</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" s="8" t="s">
         <v>71</v>
       </c>
@@ -2257,7 +2557,7 @@
         <v>-1 Treasure, +2 Food, +2 Material</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
@@ -2281,7 +2581,7 @@
         <v>+1 Food</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" hidden="1">
       <c r="A36" s="16" t="s">
         <v>90</v>
       </c>
@@ -2303,7 +2603,7 @@
         <v>For the rest of the month, Jungle, Cave, and Bog give +1 Food when used</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" hidden="1">
       <c r="A37" s="16" t="s">
         <v>105</v>
       </c>
@@ -2325,7 +2625,7 @@
         <v>Build a Jungle on Forested land, +1 Active</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" s="2" t="s">
         <v>130</v>
       </c>
@@ -2349,7 +2649,7 @@
         <v>-1 Food, +3 Food</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39" s="8" t="s">
         <v>36</v>
       </c>
@@ -2373,7 +2673,7 @@
         <v>+1 Food, +1 Active</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" hidden="1">
       <c r="A40" s="8" t="s">
         <v>48</v>
       </c>
@@ -2395,7 +2695,7 @@
         <v>Destroy 1 Freshwater to build this, +1 Food, +1 Material</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41" s="8" t="s">
         <v>59</v>
       </c>
@@ -2417,7 +2717,7 @@
         <v>-1 Material, +3 Food</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7">
       <c r="A42" s="8" t="s">
         <v>100</v>
       </c>
@@ -2439,7 +2739,7 @@
         <v>+2 Food</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" hidden="1">
       <c r="A43" s="8" t="s">
         <v>64</v>
       </c>
@@ -2461,7 +2761,7 @@
         <v>-1 Active, +1 Treasure</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7">
       <c r="A44" s="2" t="s">
         <v>34</v>
       </c>
@@ -2485,7 +2785,7 @@
         <v>+1 Material</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" hidden="1">
       <c r="A45" s="16" t="s">
         <v>88</v>
       </c>
@@ -2507,7 +2807,7 @@
         <v>Build another Rope Weaver</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" hidden="1">
       <c r="A46" s="16" t="s">
         <v>106</v>
       </c>
@@ -2529,7 +2829,7 @@
         <v>Build a Cave on Rocky land, +1 Active</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7">
       <c r="A47" s="2" t="s">
         <v>41</v>
       </c>
@@ -2553,7 +2853,7 @@
         <v>-2 Food, +1 Treasure</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7">
       <c r="A48" s="8" t="s">
         <v>98</v>
       </c>
@@ -2577,7 +2877,7 @@
         <v>-1 Food, +3 Material</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" hidden="1">
       <c r="A49" s="8" t="s">
         <v>42</v>
       </c>
@@ -2599,7 +2899,7 @@
         <v>Destroy 1 Cave to build this, +1 Treasure</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7">
       <c r="A50" s="8" t="s">
         <v>12</v>
       </c>
@@ -2621,7 +2921,7 @@
         <v>+2 Material</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" hidden="1">
       <c r="A51" s="16" t="s">
         <v>93</v>
       </c>
@@ -2643,7 +2943,7 @@
         <v>+1 Material</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7">
       <c r="A52" s="8" t="s">
         <v>62</v>
       </c>
@@ -2665,7 +2965,7 @@
         <v>+1 Treasure</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" hidden="1">
       <c r="A53" s="8" t="s">
         <v>40</v>
       </c>
@@ -2687,7 +2987,7 @@
         <v>Destroy 1 Jungle to build this, -1 Food, +3 Active</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7">
       <c r="A54" s="2" t="s">
         <v>58</v>
       </c>
@@ -2711,7 +3011,7 @@
         <v>-1 Food, +2 Active</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7">
       <c r="A55" s="8" t="s">
         <v>61</v>
       </c>
@@ -2733,7 +3033,7 @@
         <v>-1 Food, For the rest of the month, all Red developments give an additional +1 Active</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" hidden="1">
       <c r="A56" s="16" t="s">
         <v>102</v>
       </c>
@@ -2755,7 +3055,7 @@
         <v>+1 Active</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" hidden="1">
       <c r="A57" s="16" t="s">
         <v>94</v>
       </c>
@@ -2777,7 +3077,7 @@
         <v>+1 Active, Perform the effect of an adjacent development</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7">
       <c r="A58" s="2" t="s">
         <v>18</v>
       </c>
@@ -2801,7 +3101,7 @@
         <v>Destroy development, +1 Material</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7">
       <c r="A59" s="2" t="s">
         <v>144</v>
       </c>
@@ -2825,7 +3125,7 @@
         <v>-1 Food, +2 Active, +1 Material</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" hidden="1">
       <c r="A60" s="2" t="s">
         <v>19</v>
       </c>
@@ -2849,7 +3149,7 @@
         <v>-1 Food, Destroy a non-Black development, Replace with any non-Violet development</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7">
       <c r="A61" s="8" t="s">
         <v>35</v>
       </c>
@@ -2873,7 +3173,7 @@
         <v>-2 Food, +3 Active</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" hidden="1">
       <c r="A62" s="16" t="s">
         <v>97</v>
       </c>
@@ -2893,7 +3193,7 @@
         <v>Destroy 2 Black developments to build this, +1 Ship</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7">
       <c r="A63" s="8" t="s">
         <v>43</v>
       </c>
@@ -2913,7 +3213,7 @@
         <v>Destroy 1 Blue development to build this, +1 Ship</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7">
       <c r="A64" s="8" t="s">
         <v>45</v>
       </c>
@@ -2933,7 +3233,7 @@
         <v>Destroy 1 Green development to build this, +1 Ship</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" hidden="1">
       <c r="A65" s="8" t="s">
         <v>49</v>
       </c>
@@ -2953,7 +3253,7 @@
         <v>Destroy 1 Red development to build this, +2 Ships</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7">
       <c r="A66" s="8" t="s">
         <v>46</v>
       </c>
@@ -2973,7 +3273,7 @@
         <v>Destroy 1 Orange development to build this, +1 Ship</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7">
       <c r="A67" s="8" t="s">
         <v>65</v>
       </c>
@@ -2993,7 +3293,7 @@
         <v>+1 Ship</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7">
       <c r="A68" s="8" t="s">
         <v>67</v>
       </c>
@@ -3013,7 +3313,7 @@
         <v>+1 Ship</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7">
       <c r="A69" s="8" t="s">
         <v>66</v>
       </c>
@@ -3035,28 +3335,1432 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14" hidden="1" customWidth="1"/>
+    <col min="3" max="4" width="10.1640625" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="99.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8">
+        <v>0</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8">
+        <v>0</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8">
+        <v>0</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" hidden="1">
+      <c r="A22" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" hidden="1">
+      <c r="A23" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16">
+        <v>0</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G24" s="16" t="str">
+        <f ca="1">"+1 Food, +1 Material"</f>
+        <v>+1 Food, +1 Material</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="8" t="str">
+        <f ca="1">"Destroy Development, +1 Active"</f>
+        <v>Destroy Development, +1 Active</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" s="2" t="str">
+        <f ca="1">"+1 Treasure"</f>
+        <v>+1 Treasure</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" s="8" t="str">
+        <f ca="1">"-1 Treasure, +2 Food, +1 Material"</f>
+        <v>-1 Treasure, +2 Food, +1 Material</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" hidden="1">
+      <c r="A28" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G28" s="8" t="str">
+        <f ca="1">"-2 Treasure, build any development"</f>
+        <v>-2 Treasure, build any development</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" hidden="1">
+      <c r="A29" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G29" s="16" t="str">
+        <f ca="1" xml:space="preserve"> "Destroy a Black development, +2 Material"</f>
+        <v>Destroy a Black development, +2 Material</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" hidden="1">
+      <c r="A30" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" s="16" t="str">
+        <f ca="1" xml:space="preserve"> "Destroy a Black development, +3 Food"</f>
+        <v>Destroy a Black development, +3 Food</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G31" s="8" t="str">
+        <f ca="1">"-1 Material, For the rest of the month, all Blue developments give an additional +1 Treasure"</f>
+        <v>-1 Material, For the rest of the month, all Blue developments give an additional +1 Treasure</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" hidden="1">
+      <c r="A32" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" s="16" t="str">
+        <f ca="1">"Build a Base Camp on any Shore, destroy this Journey Pier"</f>
+        <v>Build a Base Camp on any Shore, destroy this Journey Pier</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G33" s="2" t="str">
+        <f ca="1">"-1 Treasure, +3 Active"</f>
+        <v>-1 Treasure, +3 Active</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G34" s="8" t="str">
+        <f ca="1">"-2 Treasure, +3 Treasure"</f>
+        <v>-2 Treasure, +3 Treasure</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G35" s="8" t="str">
+        <f ca="1">"-1 Material, +4 Food"</f>
+        <v>-1 Material, +4 Food</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" hidden="1">
+      <c r="A36" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" s="16" t="str">
+        <f ca="1">"For the rest of the month, Jungle, Cave, and Bog give +1 Food when used"</f>
+        <v>For the rest of the month, Jungle, Cave, and Bog give +1 Food when used</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" hidden="1">
+      <c r="A37" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G37" s="16" t="str">
+        <f ca="1">"Build a Jungle on Forested land, +1 Active"</f>
+        <v>Build a Jungle on Forested land, +1 Active</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G38" s="2" t="str">
+        <f ca="1">"+1 Food"</f>
+        <v>+1 Food</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39" s="2" t="str">
+        <f ca="1">"+6 Food, -1 Food for each surrounding development"</f>
+        <v>+6 Food, -1 Food for each surrounding development</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" hidden="1">
+      <c r="A40" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40" s="8" t="str">
+        <f ca="1">"Destroy 1 Freshwater to build this, +1 Food, +1 Material"</f>
+        <v>Destroy 1 Freshwater to build this, +1 Food, +1 Material</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G41" s="8" t="str">
+        <f ca="1">"+1 Food, +1 Active"</f>
+        <v>+1 Food, +1 Active</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G42" s="8" t="str">
+        <f ca="1">"-2 Material, +1 Food, +1 Treasure"</f>
+        <v>-2 Material, +1 Food, +1 Treasure</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" hidden="1">
+      <c r="A43" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" s="8" t="str">
+        <f ca="1">"-1 Active, +1 Treasure"</f>
+        <v>-1 Active, +1 Treasure</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G44" s="2" t="str">
+        <f ca="1">"+1 Material"</f>
+        <v>+1 Material</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" hidden="1">
+      <c r="A45" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G45" s="16" t="str">
+        <f ca="1">"Build another Rope Weaver"</f>
+        <v>Build another Rope Weaver</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" hidden="1">
+      <c r="A46" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F46" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G46" s="16" t="str">
+        <f ca="1">"Build a Cave on Rocky land, +1 Active"</f>
+        <v>Build a Cave on Rocky land, +1 Active</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G47" s="8" t="str">
+        <f ca="1">"+1 Material, +2 additional Material if bordering a Green development"</f>
+        <v>+1 Material, +2 additional Material if bordering a Green development</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G48" s="8" t="str">
+        <f ca="1">"+1 Material, +1 Treasure"</f>
+        <v>+1 Material, +1 Treasure</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" hidden="1">
+      <c r="A49" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G49" s="8" t="str">
+        <f ca="1">"Destroy 1 Cave to build this, +1 Treasure"</f>
+        <v>Destroy 1 Cave to build this, +1 Treasure</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G50" s="8" t="str">
+        <f ca="1">"-2 Food, +4 Material"</f>
+        <v>-2 Food, +4 Material</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" hidden="1">
+      <c r="A51" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B51" s="16"/>
+      <c r="C51" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F51" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G51" s="16" t="str">
+        <f ca="1">"+1 Material"</f>
+        <v>+1 Material</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G52" s="2" t="str">
+        <f ca="1">"-3 Food, +2 Treasure"</f>
+        <v>-3 Food, +2 Treasure</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" hidden="1">
+      <c r="A53" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E53" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F53" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G53" s="8" t="str">
+        <f ca="1">"Destroy 1 Jungle to build this, -1 Food, +3 Active"</f>
+        <v>Destroy 1 Jungle to build this, -1 Food, +3 Active</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G54" s="2" t="str">
+        <f ca="1">"-1 Food, +2 Active"</f>
+        <v>-1 Food, +2 Active</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F55" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G55" s="2" t="str">
+        <f ca="1">"Destroy development, +2 Material"</f>
+        <v>Destroy development, +2 Material</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" hidden="1">
+      <c r="A56" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="E56" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G56" s="16" t="str">
+        <f ca="1">"+1 Active"</f>
+        <v>+1 Active</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" hidden="1">
+      <c r="A57" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B57" s="16"/>
+      <c r="C57" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E57" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F57" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G57" s="16" t="str">
+        <f ca="1">"+1 Active, Perform the effect of an adjacent development"</f>
+        <v>+1 Active, Perform the effect of an adjacent development</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G58" s="8" t="str">
+        <f ca="1">"-1 Food, For the rest of the month, all Red developments give an additional +1 Active"</f>
+        <v>-1 Food, For the rest of the month, all Red developments give an additional +1 Active</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G59" s="2" t="str">
+        <f ca="1">"-1 Food, +2 Active, +1 Material"</f>
+        <v>-1 Food, +2 Active, +1 Material</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" hidden="1">
+      <c r="A60" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E60" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F60" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G60" s="2" t="str">
+        <f ca="1">"-1 Food, Destroy a non-Black development, Replace with any non-Violet development"</f>
+        <v>-1 Food, Destroy a non-Black development, Replace with any non-Violet development</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F61" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G61" s="8" t="str">
+        <f ca="1">"-2 Food, +1 Active for every two surrounding developments, rouned down"</f>
+        <v>-2 Food, +1 Active for every two surrounding developments, rouned down</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" hidden="1">
+      <c r="A62" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B62" s="16"/>
+      <c r="C62" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F62" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G62" s="16" t="str">
+        <f ca="1">"Destroy 2 Black developments to build this, +1 Ship"</f>
+        <v>Destroy 2 Black developments to build this, +1 Ship</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F63" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G63" s="8" t="str">
+        <f ca="1">"Destroy 2 Orange developments to build this, +1 Ship"</f>
+        <v>Destroy 2 Orange developments to build this, +1 Ship</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F64" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G64" s="8" t="str">
+        <f ca="1">"Destroy 2 Blue developments to build this, +1 Ship"</f>
+        <v>Destroy 2 Blue developments to build this, +1 Ship</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" hidden="1">
+      <c r="A65" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B65" s="8"/>
+      <c r="C65" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D65" s="8"/>
+      <c r="E65" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F65" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G65" s="8" t="str">
+        <f ca="1">"Destroy 1 Red development to build this, +2 Ships"</f>
+        <v>Destroy 1 Red development to build this, +2 Ships</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" s="8"/>
+      <c r="C66" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E66" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F66" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G66" s="8" t="str">
+        <f ca="1">"+1 Ship"</f>
+        <v>+1 Ship</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B67" s="8"/>
+      <c r="C67" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F67" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G67" s="8" t="str">
+        <f ca="1">"Destroy 2 Green developments to build this, +1 Ship"</f>
+        <v>Destroy 2 Green developments to build this, +1 Ship</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F68" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G68" s="8" t="str">
+        <f ca="1">"+1 Ship"</f>
+        <v>+1 Ship</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B69" s="8"/>
+      <c r="C69" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F69" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G69" s="8" t="str">
+        <f ca="1">"+1 Ship"</f>
+        <v>+1 Ship</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="19" customWidth="1"/>
-    <col min="2" max="16384" width="5.7109375" style="19"/>
+    <col min="1" max="1" width="5.6640625" style="19" customWidth="1"/>
+    <col min="2" max="16384" width="5.6640625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" ht="30" customHeight="1">
       <c r="A1" s="22">
         <v>0</v>
       </c>
@@ -3118,7 +4822,7 @@
       </c>
       <c r="AD1" s="21"/>
     </row>
-    <row r="2" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" ht="30" customHeight="1">
       <c r="A2" s="22">
         <v>-9</v>
       </c>
@@ -3213,7 +4917,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" ht="30" customHeight="1">
       <c r="A3" s="22">
         <v>-8</v>
       </c>
@@ -3303,7 +5007,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" ht="30" customHeight="1">
       <c r="A4" s="24">
         <v>-7</v>
       </c>
@@ -3398,7 +5102,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" ht="30" customHeight="1">
       <c r="A5" s="22">
         <v>-6</v>
       </c>
@@ -3488,7 +5192,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" ht="30" customHeight="1">
       <c r="A6" s="22">
         <v>-5</v>
       </c>
@@ -3583,7 +5287,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" ht="30" customHeight="1">
       <c r="A7" s="24">
         <v>-4</v>
       </c>
@@ -3673,7 +5377,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" ht="30" customHeight="1">
       <c r="A8" s="22">
         <v>-3</v>
       </c>
@@ -3768,7 +5472,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" ht="30" customHeight="1">
       <c r="A9" s="22">
         <v>-2</v>
       </c>
@@ -3858,7 +5562,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" ht="30" customHeight="1">
       <c r="A10" s="24">
         <v>-1</v>
       </c>
@@ -3953,7 +5657,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" ht="30" customHeight="1">
       <c r="A11" s="22">
         <v>0</v>
       </c>
@@ -4043,7 +5747,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" ht="30" customHeight="1">
       <c r="A12" s="24">
         <v>1</v>
       </c>
@@ -4138,7 +5842,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" ht="30" customHeight="1">
       <c r="A13" s="22">
         <v>2</v>
       </c>
@@ -4228,7 +5932,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" ht="30" customHeight="1">
       <c r="A14" s="22">
         <v>3</v>
       </c>
@@ -4323,7 +6027,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" ht="30" customHeight="1">
       <c r="A15" s="24">
         <v>4</v>
       </c>
@@ -4413,7 +6117,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" ht="30" customHeight="1">
       <c r="A16" s="22">
         <v>5</v>
       </c>
@@ -4448,7 +6152,7 @@
       <c r="AD16" s="20"/>
       <c r="AE16" s="21"/>
     </row>
-    <row r="17" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" ht="30" customHeight="1">
       <c r="A17" s="22">
         <v>6</v>
       </c>
@@ -4482,7 +6186,7 @@
       <c r="AC17" s="20"/>
       <c r="AD17" s="21"/>
     </row>
-    <row r="18" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" ht="30" customHeight="1">
       <c r="A18" s="24">
         <v>7</v>
       </c>
@@ -4517,7 +6221,7 @@
       <c r="AD18" s="20"/>
       <c r="AE18" s="21"/>
     </row>
-    <row r="19" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" ht="30" customHeight="1">
       <c r="A19" s="22">
         <v>8</v>
       </c>
@@ -4551,7 +6255,7 @@
       <c r="AC19" s="20"/>
       <c r="AD19" s="21"/>
     </row>
-    <row r="20" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" ht="30" customHeight="1">
       <c r="A20" s="22">
         <v>9</v>
       </c>
@@ -4586,11 +6290,11 @@
       <c r="AD20" s="20"/>
       <c r="AE20" s="21"/>
     </row>
-    <row r="30" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" ht="30" customHeight="1">
       <c r="J30" s="25"/>
       <c r="O30" s="25"/>
     </row>
-    <row r="31" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" ht="30" customHeight="1">
       <c r="J31" s="30"/>
       <c r="K31" s="20">
         <v>-9</v>
@@ -4606,7 +6310,7 @@
       </c>
       <c r="O31" s="31"/>
     </row>
-    <row r="32" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" ht="30" customHeight="1">
       <c r="J32" s="20">
         <v>-8</v>
       </c>
@@ -4626,7 +6330,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="10:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="10:18" ht="30" customHeight="1">
       <c r="J33" s="33"/>
       <c r="K33" s="20">
         <v>-7</v>
@@ -4645,14 +6349,14 @@
         <v>117</v>
       </c>
     </row>
-    <row r="34" spans="10:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="10:18" ht="30" customHeight="1">
       <c r="J34" s="32"/>
       <c r="O34" s="26"/>
       <c r="R34" s="19" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="10:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="10:18" ht="30" customHeight="1">
       <c r="J35" s="29"/>
       <c r="K35" s="20">
         <v>-8</v>
@@ -4671,7 +6375,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="10:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="10:18" ht="30" customHeight="1">
       <c r="J36" s="20">
         <v>-7</v>
       </c>
@@ -4694,7 +6398,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="10:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="10:18" ht="30" customHeight="1">
       <c r="J37" s="35"/>
       <c r="K37" s="20">
         <v>-6</v>
@@ -4710,17 +6414,21 @@
       </c>
       <c r="O37" s="34"/>
     </row>
-    <row r="38" spans="10:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="10:18" ht="30" customHeight="1">
       <c r="J38" s="26"/>
       <c r="O38" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -4728,9 +6436,9 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>107</v>
       </c>
@@ -4738,7 +6446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>108</v>
       </c>
@@ -4746,7 +6454,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="B4" t="s">
         <v>115</v>
       </c>
@@ -4754,45 +6462,45 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>109</v>
       </c>
       <c r="B5">
-        <f>0.5*width</f>
+        <f ca="1">0.5*width</f>
         <v>1.5</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>110</v>
       </c>
       <c r="B6">
-        <f>(0.5*width-0.5*height)</f>
+        <f ca="1">(0.5*width-0.5*height)</f>
         <v>0.75</v>
       </c>
       <c r="C6">
-        <f>-0.5*height</f>
+        <f ca="1">-0.5*height</f>
         <v>-0.75</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>111</v>
       </c>
       <c r="B7">
-        <f>-(0.5*width-0.5*height)</f>
+        <f ca="1">-(0.5*width-0.5*height)</f>
         <v>-0.75</v>
       </c>
       <c r="C7">
-        <f>-0.5*height</f>
+        <f ca="1">-0.5*height</f>
         <v>-0.75</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>112</v>
       </c>
@@ -4803,39 +6511,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>113</v>
       </c>
       <c r="B9">
-        <f>-(0.5*width-0.5*height)</f>
+        <f ca="1">-(0.5*width-0.5*height)</f>
         <v>-0.75</v>
       </c>
       <c r="C9">
-        <f>0.5*height</f>
+        <f ca="1">0.5*height</f>
         <v>0.75</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>114</v>
       </c>
       <c r="B10">
-        <f>(0.5*width-0.5*height)</f>
+        <f ca="1">(0.5*width-0.5*height)</f>
         <v>0.75</v>
       </c>
       <c r="C10">
-        <f>0.5*height</f>
+        <f ca="1">0.5*height</f>
         <v>0.75</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -4843,20 +6556,20 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="4" style="44" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44" style="45" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="44"/>
+    <col min="3" max="16384" width="8.83203125" style="44"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18">
       <c r="A1" s="51" t="s">
         <v>133</v>
       </c>
       <c r="B1" s="51"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="48">
         <v>1</v>
       </c>
@@ -4864,7 +6577,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="48">
         <v>2</v>
       </c>
@@ -4872,7 +6585,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="28">
       <c r="A4" s="48">
         <v>3</v>
       </c>
@@ -4880,7 +6593,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="28">
       <c r="A5" s="46">
         <v>3.1</v>
       </c>
@@ -4888,7 +6601,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="46">
         <v>3.2</v>
       </c>
@@ -4896,7 +6609,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="28">
       <c r="A7" s="46">
         <v>3.3</v>
       </c>
@@ -4904,7 +6617,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="28">
       <c r="A8" s="46">
         <v>3.4</v>
       </c>
@@ -4912,7 +6625,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="28">
       <c r="A9" s="46">
         <v>3.5</v>
       </c>
@@ -4920,7 +6633,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="28">
       <c r="A10" s="48">
         <v>4</v>
       </c>
@@ -4928,7 +6641,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="28">
       <c r="A11" s="48">
         <v>5</v>
       </c>
@@ -4941,28 +6654,32 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="44" customWidth="1"/>
-    <col min="4" max="4" width="2.85546875" customWidth="1"/>
-    <col min="5" max="5" width="70.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="2.83203125" customWidth="1"/>
+    <col min="3" max="3" width="46" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" customWidth="1"/>
+    <col min="5" max="5" width="70.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="50" t="s">
         <v>149</v>
       </c>
@@ -4974,7 +6691,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>152</v>
       </c>
@@ -4985,7 +6702,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>153</v>
       </c>
@@ -4993,21 +6710,21 @@
         <v>155</v>
       </c>
       <c r="E3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>157</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>158</v>
       </c>
@@ -5015,10 +6732,10 @@
         <v>156</v>
       </c>
       <c r="E5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>159</v>
       </c>
@@ -5027,10 +6744,10 @@
         <v>-# Actions, +# Actions</v>
       </c>
       <c r="E6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -5038,10 +6755,10 @@
         <v>165</v>
       </c>
       <c r="E7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>161</v>
       </c>
@@ -5049,75 +6766,88 @@
         <v>172</v>
       </c>
       <c r="E8" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>162</v>
       </c>
       <c r="C9" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>164</v>
       </c>
       <c r="C10" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>163</v>
       </c>
       <c r="C11" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Player bar, development destruction effects, cosmetic changes
</commit_message>
<xml_diff>
--- a/SettleGame.xlsx
+++ b/SettleGame.xlsx
@@ -1548,11 +1548,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2145997192"/>
-        <c:axId val="2145994776"/>
+        <c:axId val="2088664840"/>
+        <c:axId val="2088667912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2145997192"/>
+        <c:axId val="2088664840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1562,12 +1562,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145994776"/>
+        <c:crossAx val="2088667912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2145994776"/>
+        <c:axId val="2088667912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1578,7 +1578,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145997192"/>
+        <c:crossAx val="2088664840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3354,8 +3354,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3787,8 +3787,8 @@
         <v>30</v>
       </c>
       <c r="G27" s="8" t="str">
-        <f ca="1">"-1 Treasure, +2 Food, +1 Material"</f>
-        <v>-1 Treasure, +2 Food, +1 Material</v>
+        <f ca="1">"-1 Treasure, +2 Food, +2 Material"</f>
+        <v>-1 Treasure, +2 Food, +2 Material</v>
       </c>
     </row>
     <row r="28" spans="1:7" hidden="1">
@@ -4561,8 +4561,8 @@
         <v>29</v>
       </c>
       <c r="G61" s="8" t="str">
-        <f ca="1">"-2 Food, +1 Active for every two surrounding developments, rounded up"</f>
-        <v>-2 Food, +1 Active for every two surrounding developments, rounded up</v>
+        <f ca="1">"-2 Food; +1 Active, +1 Material for every two surrounding developments, rounded up"</f>
+        <v>-2 Food; +1 Active, +1 Material for every two surrounding developments, rounded up</v>
       </c>
     </row>
     <row r="62" spans="1:7" hidden="1">

</xml_diff>

<commit_message>
Minor graphical changes, continuation of banner visual effect
</commit_message>
<xml_diff>
--- a/SettleGame.xlsx
+++ b/SettleGame.xlsx
@@ -1548,11 +1548,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2088664840"/>
-        <c:axId val="2088667912"/>
+        <c:axId val="2142003880"/>
+        <c:axId val="2142006856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2088664840"/>
+        <c:axId val="2142003880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1562,12 +1562,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088667912"/>
+        <c:crossAx val="2142006856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2088667912"/>
+        <c:axId val="2142006856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1578,7 +1578,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088664840"/>
+        <c:crossAx val="2142003880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3355,7 +3355,7 @@
   <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3967,8 +3967,8 @@
         <v>28</v>
       </c>
       <c r="G35" s="8" t="str">
-        <f ca="1">"-1 Material, +4 Food"</f>
-        <v>-1 Material, +4 Food</v>
+        <f ca="1">"+3 Food, +1 Material"</f>
+        <v>+3 Food, +1 Material</v>
       </c>
     </row>
     <row r="36" spans="1:7" hidden="1">
@@ -4059,8 +4059,8 @@
         <v>28</v>
       </c>
       <c r="G39" s="2" t="str">
-        <f ca="1">"+6 Food, -1 Food for each surrounding development"</f>
-        <v>+6 Food, -1 Food for each surrounding development</v>
+        <f ca="1">"+5 Food, -1 Food for each surrounding development"</f>
+        <v>+5 Food, -1 Food for each surrounding development</v>
       </c>
     </row>
     <row r="40" spans="1:7" hidden="1">

</xml_diff>